<commit_message>
Avoid warning in trans/AVLo (#174)
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BD2AED-0597-43CE-962E-8ADB635679A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C91C1FE-2F2E-4D14-8A9C-BB9A8C58315F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19875" yWindow="480" windowWidth="25935" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="150" windowWidth="25935" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2662,7 +2662,7 @@
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="45">
+    <row r="1" spans="1:37" ht="30">
       <c r="A1" s="19" t="s">
         <v>105</v>
       </c>
@@ -3810,6 +3810,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AK8">
+        <f t="shared" ref="AK8:AK13" si="2">$B8</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
@@ -3954,6 +3958,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="AK9">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="1" t="s">
@@ -4088,15 +4096,19 @@
         <v>41.989116133258747</v>
       </c>
       <c r="AH10" s="6">
-        <f t="shared" ref="AH10:BN13" si="2">$B10</f>
+        <f t="shared" ref="AH10:AK10" si="3">$B10</f>
         <v>41.989116133258747</v>
       </c>
       <c r="AI10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41.989116133258747</v>
       </c>
       <c r="AJ10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AK10" s="6">
+        <f t="shared" si="3"/>
         <v>41.989116133258747</v>
       </c>
     </row>
@@ -4173,75 +4185,79 @@
         <v>3512.35916421195</v>
       </c>
       <c r="S11" s="6">
-        <f t="shared" ref="S11:AY13" si="3">$B11</f>
+        <f t="shared" ref="S11:AK13" si="4">$B11</f>
         <v>3512.35916421195</v>
       </c>
       <c r="T11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="U11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="V11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="W11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="X11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="Y11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="Z11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AA11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AB11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AC11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AD11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AE11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AF11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AG11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AH11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AI11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
       <c r="AJ11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AK11" s="6">
+        <f t="shared" si="4"/>
         <v>3512.35916421195</v>
       </c>
     </row>
@@ -4318,75 +4334,79 @@
         <v>1974.4736422180429</v>
       </c>
       <c r="S12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="T12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="U12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="V12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="W12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="X12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="Y12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="Z12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AA12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AB12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AC12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AD12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AE12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AF12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AG12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AH12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AI12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
       <c r="AJ12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AK12" s="6">
+        <f t="shared" si="4"/>
         <v>1974.4736422180429</v>
       </c>
     </row>
@@ -4462,75 +4482,79 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct AVLo for passenger rail
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\AVLo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A75BC0-CB70-4CB5-9D67-E3CEE4D29F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -28,12 +29,23 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -372,12 +384,21 @@
   </si>
   <si>
     <t>Vehicle Loading (tons)</t>
+  </si>
+  <si>
+    <t>The units for rail in the BTS data set are unclear whether they report locomotive-miles or train-car-miles. Based on the</t>
+  </si>
+  <si>
+    <t>scale, we assume the units are train-car-miles.</t>
+  </si>
+  <si>
+    <t>Assumption - train cars per locomotive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1245,7 +1266,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1278,162 +1299,163 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="154">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="3"/>
-    <cellStyle name="20% - Accent3 2" xfId="4"/>
-    <cellStyle name="20% - Accent4 2" xfId="5"/>
-    <cellStyle name="20% - Accent5 2" xfId="6"/>
-    <cellStyle name="20% - Accent6 2" xfId="7"/>
-    <cellStyle name="40% - Accent1 2" xfId="8"/>
-    <cellStyle name="40% - Accent2 2" xfId="9"/>
-    <cellStyle name="40% - Accent3 2" xfId="10"/>
-    <cellStyle name="40% - Accent4 2" xfId="11"/>
-    <cellStyle name="40% - Accent5 2" xfId="12"/>
-    <cellStyle name="40% - Accent6 2" xfId="13"/>
-    <cellStyle name="60% - Accent1 2" xfId="14"/>
-    <cellStyle name="60% - Accent2 2" xfId="15"/>
-    <cellStyle name="60% - Accent3 2" xfId="16"/>
-    <cellStyle name="60% - Accent4 2" xfId="17"/>
-    <cellStyle name="60% - Accent5 2" xfId="18"/>
-    <cellStyle name="60% - Accent6 2" xfId="19"/>
-    <cellStyle name="Accent1 2" xfId="20"/>
-    <cellStyle name="Accent2 2" xfId="21"/>
-    <cellStyle name="Accent3 2" xfId="22"/>
-    <cellStyle name="Accent4 2" xfId="23"/>
-    <cellStyle name="Accent5 2" xfId="24"/>
-    <cellStyle name="Accent6 2" xfId="25"/>
-    <cellStyle name="Bad 2" xfId="26"/>
-    <cellStyle name="Body: normal cell" xfId="27"/>
-    <cellStyle name="Body: normal cell 2" xfId="28"/>
-    <cellStyle name="Calculation 2" xfId="29"/>
-    <cellStyle name="Check Cell 2" xfId="30"/>
-    <cellStyle name="Column heading" xfId="31"/>
-    <cellStyle name="Comma 2" xfId="32"/>
-    <cellStyle name="Comma 2 2" xfId="33"/>
-    <cellStyle name="Comma 3" xfId="34"/>
-    <cellStyle name="Comma 4" xfId="35"/>
-    <cellStyle name="Comma 5" xfId="36"/>
-    <cellStyle name="Comma 6" xfId="37"/>
-    <cellStyle name="Comma 7" xfId="38"/>
-    <cellStyle name="Comma 8" xfId="39"/>
-    <cellStyle name="Corner heading" xfId="40"/>
-    <cellStyle name="Currency 2" xfId="41"/>
-    <cellStyle name="Currency 3" xfId="42"/>
-    <cellStyle name="Currency 3 2" xfId="43"/>
-    <cellStyle name="Data" xfId="44"/>
-    <cellStyle name="Data 2" xfId="45"/>
-    <cellStyle name="Data no deci" xfId="46"/>
-    <cellStyle name="Data Superscript" xfId="47"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="48"/>
-    <cellStyle name="Explanatory Text 2" xfId="49"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="50"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="51"/>
-    <cellStyle name="Footnotes: top row" xfId="52"/>
-    <cellStyle name="Footnotes: top row 2" xfId="53"/>
-    <cellStyle name="Good 2" xfId="54"/>
-    <cellStyle name="Header: bottom row" xfId="55"/>
-    <cellStyle name="Header: bottom row 2" xfId="56"/>
-    <cellStyle name="Heading 1 2" xfId="57"/>
-    <cellStyle name="Heading 2 2" xfId="58"/>
-    <cellStyle name="Heading 3 2" xfId="59"/>
-    <cellStyle name="Heading 4 2" xfId="60"/>
-    <cellStyle name="Hed Side" xfId="61"/>
-    <cellStyle name="Hed Side 2" xfId="62"/>
-    <cellStyle name="Hed Side bold" xfId="63"/>
-    <cellStyle name="Hed Side Indent" xfId="64"/>
-    <cellStyle name="Hed Side Regular" xfId="65"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="66"/>
-    <cellStyle name="Hed Top" xfId="67"/>
-    <cellStyle name="Hed Top - SECTION" xfId="68"/>
-    <cellStyle name="Hed Top_3-new4" xfId="69"/>
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Body: normal cell" xfId="27" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Calculation 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Check Cell 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Column heading" xfId="31" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Comma 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Comma 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 4" xfId="35" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 5" xfId="36" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 6" xfId="37" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 7" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 8" xfId="39" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Corner heading" xfId="40" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Currency 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Currency 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Currency 3 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Data" xfId="44" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Data 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Data no deci" xfId="46" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Data Superscript" xfId="47" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="48" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="50" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="52" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Good 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Header: bottom row" xfId="55" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Heading 1 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Heading 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Heading 3 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Heading 4 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Hed Side" xfId="61" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Hed Side 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Hed Side bold" xfId="63" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="64" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="65" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Hed Top" xfId="67" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Hed Top - SECTION" xfId="68" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Hed Top_3-new4" xfId="69" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="70"/>
-    <cellStyle name="Input 2" xfId="71"/>
-    <cellStyle name="Linked Cell 2" xfId="72"/>
-    <cellStyle name="Neutral 2" xfId="73"/>
+    <cellStyle name="Hyperlink 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Input 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Neutral 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="74"/>
-    <cellStyle name="Normal 11" xfId="75"/>
-    <cellStyle name="Normal 2" xfId="76"/>
-    <cellStyle name="Normal 2 2" xfId="77"/>
-    <cellStyle name="Normal 2 3" xfId="78"/>
-    <cellStyle name="Normal 3" xfId="79"/>
-    <cellStyle name="Normal 3 2" xfId="80"/>
-    <cellStyle name="Normal 3 2 2" xfId="81"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="82"/>
-    <cellStyle name="Normal 3 2 3" xfId="83"/>
-    <cellStyle name="Normal 3 3" xfId="84"/>
-    <cellStyle name="Normal 3 3 2" xfId="85"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="86"/>
-    <cellStyle name="Normal 3 3 3" xfId="87"/>
-    <cellStyle name="Normal 3 4" xfId="88"/>
-    <cellStyle name="Normal 3 4 2" xfId="89"/>
-    <cellStyle name="Normal 3 5" xfId="90"/>
-    <cellStyle name="Normal 3 6" xfId="91"/>
-    <cellStyle name="Normal 3 7" xfId="92"/>
-    <cellStyle name="Normal 4" xfId="93"/>
-    <cellStyle name="Normal 4 2" xfId="94"/>
-    <cellStyle name="Normal 4 2 2" xfId="95"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="96"/>
-    <cellStyle name="Normal 4 2 3" xfId="97"/>
-    <cellStyle name="Normal 4 3" xfId="98"/>
-    <cellStyle name="Normal 4 3 2" xfId="99"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="100"/>
-    <cellStyle name="Normal 4 3 3" xfId="101"/>
-    <cellStyle name="Normal 4 4" xfId="102"/>
-    <cellStyle name="Normal 4 4 2" xfId="103"/>
-    <cellStyle name="Normal 4 5" xfId="104"/>
-    <cellStyle name="Normal 4 6" xfId="105"/>
-    <cellStyle name="Normal 4 7" xfId="106"/>
-    <cellStyle name="Normal 5" xfId="107"/>
-    <cellStyle name="Normal 5 2" xfId="108"/>
-    <cellStyle name="Normal 5 3" xfId="109"/>
-    <cellStyle name="Normal 6" xfId="110"/>
-    <cellStyle name="Normal 6 2" xfId="111"/>
-    <cellStyle name="Normal 7" xfId="112"/>
-    <cellStyle name="Normal 7 2" xfId="113"/>
-    <cellStyle name="Normal 8" xfId="114"/>
-    <cellStyle name="Normal 9" xfId="115"/>
-    <cellStyle name="Note 2" xfId="116"/>
-    <cellStyle name="Note 2 2" xfId="117"/>
-    <cellStyle name="Output 2" xfId="118"/>
-    <cellStyle name="Parent row" xfId="119"/>
-    <cellStyle name="Parent row 2" xfId="120"/>
-    <cellStyle name="Percent 2" xfId="121"/>
-    <cellStyle name="Percent 2 2" xfId="122"/>
-    <cellStyle name="Percent 3" xfId="123"/>
-    <cellStyle name="Percent 3 2" xfId="124"/>
-    <cellStyle name="Percent 4" xfId="125"/>
-    <cellStyle name="Reference" xfId="126"/>
-    <cellStyle name="Row heading" xfId="127"/>
-    <cellStyle name="Source Hed" xfId="128"/>
-    <cellStyle name="Source Letter" xfId="129"/>
-    <cellStyle name="Source Superscript" xfId="130"/>
-    <cellStyle name="Source Superscript 2" xfId="131"/>
-    <cellStyle name="Source Text" xfId="132"/>
-    <cellStyle name="Source Text 2" xfId="133"/>
-    <cellStyle name="State" xfId="134"/>
-    <cellStyle name="Superscript" xfId="135"/>
-    <cellStyle name="Table Data" xfId="136"/>
-    <cellStyle name="Table Head Top" xfId="137"/>
-    <cellStyle name="Table Hed Side" xfId="138"/>
-    <cellStyle name="Table title" xfId="139"/>
-    <cellStyle name="Table title 2" xfId="140"/>
-    <cellStyle name="Title 2" xfId="141"/>
-    <cellStyle name="Title Text" xfId="142"/>
-    <cellStyle name="Title Text 1" xfId="143"/>
-    <cellStyle name="Title Text 2" xfId="144"/>
-    <cellStyle name="Title-1" xfId="145"/>
-    <cellStyle name="Title-2" xfId="146"/>
-    <cellStyle name="Title-3" xfId="147"/>
-    <cellStyle name="Total 2" xfId="148"/>
-    <cellStyle name="Warning Text 2" xfId="149"/>
-    <cellStyle name="Wrap" xfId="150"/>
-    <cellStyle name="Wrap Bold" xfId="151"/>
-    <cellStyle name="Wrap Title" xfId="152"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="153"/>
+    <cellStyle name="Normal 10" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 11" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 3 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 3 4" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 3 5" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 3 6" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 3 7" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 4" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 4 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 4 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 4 3 3" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 4 4" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 4 4 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 4 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 4 6" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 4 7" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 7 2" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 8" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 9" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Note 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Note 2 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Output 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Parent row" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Table title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Table title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Title 2" xfId="141" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Title Text" xfId="142" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Title Text 1" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Title Text 2" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Title-1" xfId="145" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Title-2" xfId="146" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Title-3" xfId="147" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Total 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Warning Text 2" xfId="149" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Wrap" xfId="150" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Wrap Bold" xfId="151" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Wrap Title" xfId="152" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="153" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1605,6 +1627,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1640,6 +1679,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1815,17 +1871,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" customWidth="1"/>
-    <col min="2" max="2" width="85.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="85.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2061,18 +2117,28 @@
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -2080,16 +2146,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="73.59765625" customWidth="1"/>
+    <col min="1" max="1" width="73.6328125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.265625" customWidth="1"/>
+    <col min="3" max="3" width="102.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2245,361 +2313,366 @@
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:3" s="11" customFormat="1">
+      <c r="A22" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B23" s="12">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
-        <v>5914</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>5914</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="6">
-        <f>B24/B23</f>
+      <c r="B26" s="6">
+        <f>B25/B24</f>
         <v>155.63157894736841</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B27" s="12">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="6">
-        <v>16805</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6">
-        <v>2196</v>
+        <v>16805</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="6">
-        <v>11129</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6">
-        <v>685</v>
+        <v>11129</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6">
-        <v>90</v>
+        <v>685</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6">
-        <v>337</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="6">
-        <f>B27/B30</f>
-        <v>24.532846715328468</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="6">
-        <f t="shared" ref="B34:B35" si="0">B28/B31</f>
-        <v>24.4</v>
+        <f>B28/B31</f>
+        <v>24.532846715328468</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="6">
+        <f t="shared" ref="B35:B36" si="0">B29/B32</f>
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B36" s="6">
         <f t="shared" si="0"/>
         <v>33.023738872403563</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="6">
-        <f>(B25*B24+B33*B27+B34*B28+B35*B29)/SUM(B24,B27:B29)</f>
-        <v>48.656731685074099</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
+      <c r="B37" s="6">
+        <f>(B26*B25+B34*B28+B35*B29+B36*B30)/SUM(B25,B28:B30)*B22</f>
+        <v>486.56731685074101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>2005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="15">
-        <v>2967</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="15">
-        <v>100</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B41" s="15">
-        <v>27876</v>
-      </c>
-      <c r="C41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="15">
+        <v>27876</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B43" s="15">
         <v>4151</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="15"/>
-      <c r="C43" t="s">
+    <row r="44" spans="1:3">
+      <c r="B44" s="15"/>
+      <c r="C44" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="15">
-        <v>6614973</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="15">
-        <v>5727512</v>
+        <v>6614973</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B46" s="15">
-        <v>44777151</v>
+        <v>5727512</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="15">
+        <v>44777151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B48" s="15">
         <v>12172542</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="B48" s="15"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2">
+      <c r="B49" s="15"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="15">
-        <f>B44/B39</f>
-        <v>2229.5156723963601</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>94</v>
       </c>
       <c r="B50" s="15">
         <f>B45/B40</f>
+        <v>2229.5156723963601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="15">
+        <f>B46/B41</f>
         <v>57275.12</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="15">
-        <f t="shared" ref="B51:B52" si="1">B46/B41</f>
+      <c r="B52" s="15">
+        <f t="shared" ref="B52:B53" si="1">B47/B42</f>
         <v>1606.2975678002583</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B53" s="15">
         <f t="shared" si="1"/>
         <v>2932.4360395085523</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2">
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="15">
-        <f>SUMPRODUCT(B39:B42,B49:B52)/SUM(B39:B42)</f>
+      <c r="B55" s="15">
+        <f>SUMPRODUCT(B40:B43,B50:B53)/SUM(B40:B43)</f>
         <v>1974.4736422180429</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="6"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:2">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B57" s="13">
         <v>2007</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>13611</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="11" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B59" s="11">
         <v>17287</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="10" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="7">
-        <f>B58/B57</f>
+      <c r="B60" s="7">
+        <f>B59/B58</f>
         <v>1.2700756740871355</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="10"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B62" s="4">
         <v>2007</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B63" s="11">
         <v>1670994</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B64" s="6">
         <v>2640170</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="7">
-        <f>B63/B62</f>
+      <c r="B65" s="7">
+        <f>B64/B63</f>
         <v>1.579999688807979</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C65" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="1:3">
       <c r="B66" s="6"/>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="9"/>
+    <row r="67" spans="1:3">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B36" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -2607,13 +2680,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="42.75">
+    <row r="1" spans="1:37" ht="43.5">
       <c r="A1" s="19" t="s">
         <v>111</v>
       </c>
@@ -3177,148 +3250,148 @@
         <v>15</v>
       </c>
       <c r="B5" s="9">
-        <f>'BTS NTS Modal Profile Data'!B36</f>
-        <v>48.656731685074099</v>
+        <f>'BTS NTS Modal Profile Data'!B37</f>
+        <v>486.56731685074101</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
       <c r="AK5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>486.56731685074101</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -3474,7 +3547,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="7">
-        <f>'BTS NTS Modal Profile Data'!B59</f>
+        <f>'BTS NTS Modal Profile Data'!B60</f>
         <v>1.2700756740871355</v>
       </c>
       <c r="C7" s="7">
@@ -3624,7 +3697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -3632,12 +3705,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="42.75">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="43.5">
       <c r="A1" s="19" t="s">
         <v>112</v>
       </c>
@@ -4330,7 +4403,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6">
-        <f>'BTS NTS Modal Profile Data'!B54</f>
+        <f>'BTS NTS Modal Profile Data'!B55</f>
         <v>1974.4736422180429</v>
       </c>
       <c r="C6" s="6">

</xml_diff>

<commit_message>
Adjust loading for passenger HDVs to reflect COVID dip
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A75BC0-CB70-4CB5-9D67-E3CEE4D29F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142A8458-B38E-42D5-80D8-6041B2C122C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BTS NTS Modal Profile Data" sheetId="3" r:id="rId2"/>
-    <sheet name="AVLo-passengers" sheetId="2" r:id="rId3"/>
-    <sheet name="AVLo-freight" sheetId="4" r:id="rId4"/>
+    <sheet name="BCDTRtSY" sheetId="5" r:id="rId3"/>
+    <sheet name="AVLo-passengers" sheetId="2" r:id="rId4"/>
+    <sheet name="AVLo-freight" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Eno_TM">'[1]1997  Table 1a Modified'!#REF!</definedName>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -393,6 +395,15 @@
   </si>
   <si>
     <t>Assumption - train cars per locomotive</t>
+  </si>
+  <si>
+    <t>Cargo Dist Transported Relative to Start Year (dimensionless)</t>
+  </si>
+  <si>
+    <t>For buses, we adjust the loading by the values in trans/BCDTRtSY to reflect the fact that passenger bus</t>
+  </si>
+  <si>
+    <t>loading dipped due to the COVID-19 pandemic.</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1277,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1284,14 +1295,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1299,7 +1307,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="154">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1546,6 +1553,3276 @@
       <sheetData sheetId="32"/>
       <sheetData sheetId="33"/>
       <sheetData sheetId="34"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="AEO 2020 7"/>
+      <sheetName val="AEO 2020 36"/>
+      <sheetName val="AEO 2020 46"/>
+      <sheetName val="AEO 2020 47"/>
+      <sheetName val="AEO 2020 49"/>
+      <sheetName val="AEO 2021 7"/>
+      <sheetName val="AEO 2021 35"/>
+      <sheetName val="AEO 2021 46"/>
+      <sheetName val="AEO 2021 47"/>
+      <sheetName val="AEO 2021 49"/>
+      <sheetName val="AEO 2022 7"/>
+      <sheetName val="AEO 2022 35 Raw"/>
+      <sheetName val="AEO 2022 35"/>
+      <sheetName val="AEO 2022 46 Raw"/>
+      <sheetName val="AEO 2022 46"/>
+      <sheetName val="AEO 2022 47 Raw"/>
+      <sheetName val="AEO 2022 47"/>
+      <sheetName val="AEO 2022 49 Raw"/>
+      <sheetName val="AEO 2022 49"/>
+      <sheetName val="aircraft calibration"/>
+      <sheetName val="BCDTRtSY-psgr"/>
+      <sheetName val="BCDTRtSY-frgt"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>highogs.d112619a</v>
+          </cell>
+          <cell r="C1">
+            <v>2019</v>
+          </cell>
+          <cell r="D1">
+            <v>2020</v>
+          </cell>
+          <cell r="E1">
+            <v>2021</v>
+          </cell>
+          <cell r="F1">
+            <v>2022</v>
+          </cell>
+          <cell r="G1">
+            <v>2023</v>
+          </cell>
+          <cell r="H1">
+            <v>2024</v>
+          </cell>
+          <cell r="I1">
+            <v>2025</v>
+          </cell>
+          <cell r="J1">
+            <v>2026</v>
+          </cell>
+          <cell r="K1">
+            <v>2027</v>
+          </cell>
+          <cell r="L1">
+            <v>2028</v>
+          </cell>
+          <cell r="M1">
+            <v>2029</v>
+          </cell>
+          <cell r="N1">
+            <v>2030</v>
+          </cell>
+          <cell r="O1">
+            <v>2031</v>
+          </cell>
+          <cell r="P1">
+            <v>2032</v>
+          </cell>
+          <cell r="Q1">
+            <v>2033</v>
+          </cell>
+          <cell r="R1">
+            <v>2034</v>
+          </cell>
+          <cell r="S1">
+            <v>2035</v>
+          </cell>
+          <cell r="T1">
+            <v>2036</v>
+          </cell>
+          <cell r="U1">
+            <v>2037</v>
+          </cell>
+          <cell r="V1">
+            <v>2038</v>
+          </cell>
+          <cell r="W1">
+            <v>2039</v>
+          </cell>
+          <cell r="X1">
+            <v>2040</v>
+          </cell>
+          <cell r="Y1">
+            <v>2041</v>
+          </cell>
+          <cell r="Z1">
+            <v>2042</v>
+          </cell>
+          <cell r="AA1">
+            <v>2043</v>
+          </cell>
+          <cell r="AB1">
+            <v>2044</v>
+          </cell>
+          <cell r="AC1">
+            <v>2045</v>
+          </cell>
+          <cell r="AD1">
+            <v>2046</v>
+          </cell>
+          <cell r="AE1">
+            <v>2047</v>
+          </cell>
+          <cell r="AF1">
+            <v>2048</v>
+          </cell>
+          <cell r="AG1">
+            <v>2049</v>
+          </cell>
+          <cell r="AH1">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>TKI000:ba_Light-DutyVeh</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v xml:space="preserve">   Light-Duty Vehicles less than 8,501 pounds</v>
+          </cell>
+          <cell r="C18">
+            <v>2917.2534179999998</v>
+          </cell>
+          <cell r="D18">
+            <v>2975.1254880000001</v>
+          </cell>
+          <cell r="E18">
+            <v>3025.3583979999999</v>
+          </cell>
+          <cell r="F18">
+            <v>3062.7468260000001</v>
+          </cell>
+          <cell r="G18">
+            <v>3083.977539</v>
+          </cell>
+          <cell r="H18">
+            <v>3096.5910640000002</v>
+          </cell>
+          <cell r="I18">
+            <v>3105.9812010000001</v>
+          </cell>
+          <cell r="J18">
+            <v>3125.5920409999999</v>
+          </cell>
+          <cell r="K18">
+            <v>3146.880615</v>
+          </cell>
+          <cell r="L18">
+            <v>3167.633057</v>
+          </cell>
+          <cell r="M18">
+            <v>3188.2370609999998</v>
+          </cell>
+          <cell r="N18">
+            <v>3209.845703</v>
+          </cell>
+          <cell r="O18">
+            <v>3233.3459469999998</v>
+          </cell>
+          <cell r="P18">
+            <v>3252.6281739999999</v>
+          </cell>
+          <cell r="Q18">
+            <v>3271.139404</v>
+          </cell>
+          <cell r="R18">
+            <v>3285.1403810000002</v>
+          </cell>
+          <cell r="S18">
+            <v>3295.6909179999998</v>
+          </cell>
+          <cell r="T18">
+            <v>3311.9399410000001</v>
+          </cell>
+          <cell r="U18">
+            <v>3327.9958499999998</v>
+          </cell>
+          <cell r="V18">
+            <v>3344.2626949999999</v>
+          </cell>
+          <cell r="W18">
+            <v>3361.544922</v>
+          </cell>
+          <cell r="X18">
+            <v>3379.7543949999999</v>
+          </cell>
+          <cell r="Y18">
+            <v>3396.2570799999999</v>
+          </cell>
+          <cell r="Z18">
+            <v>3413.8405760000001</v>
+          </cell>
+          <cell r="AA18">
+            <v>3432.0297850000002</v>
+          </cell>
+          <cell r="AB18">
+            <v>3451.1577149999998</v>
+          </cell>
+          <cell r="AC18">
+            <v>3472.0922850000002</v>
+          </cell>
+          <cell r="AD18">
+            <v>3496.9057619999999</v>
+          </cell>
+          <cell r="AE18">
+            <v>3524.3183589999999</v>
+          </cell>
+          <cell r="AF18">
+            <v>3555.436768</v>
+          </cell>
+          <cell r="AG18">
+            <v>3588.8325199999999</v>
+          </cell>
+          <cell r="AH18">
+            <v>3624.4035640000002</v>
+          </cell>
+          <cell r="AI18">
+            <v>7.0260000000000001E-3</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>TKI000:buspassmiles</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v xml:space="preserve">   Bus Transportation</v>
+          </cell>
+          <cell r="C22">
+            <v>210.13850400000001</v>
+          </cell>
+          <cell r="D22">
+            <v>211.126205</v>
+          </cell>
+          <cell r="E22">
+            <v>212.116165</v>
+          </cell>
+          <cell r="F22">
+            <v>213.08595299999999</v>
+          </cell>
+          <cell r="G22">
+            <v>214.01353499999999</v>
+          </cell>
+          <cell r="H22">
+            <v>214.96095299999999</v>
+          </cell>
+          <cell r="I22">
+            <v>215.98413099999999</v>
+          </cell>
+          <cell r="J22">
+            <v>216.989777</v>
+          </cell>
+          <cell r="K22">
+            <v>217.98005699999999</v>
+          </cell>
+          <cell r="L22">
+            <v>218.98109400000001</v>
+          </cell>
+          <cell r="M22">
+            <v>219.96804800000001</v>
+          </cell>
+          <cell r="N22">
+            <v>220.90673799999999</v>
+          </cell>
+          <cell r="O22">
+            <v>221.807053</v>
+          </cell>
+          <cell r="P22">
+            <v>222.678833</v>
+          </cell>
+          <cell r="Q22">
+            <v>223.455963</v>
+          </cell>
+          <cell r="R22">
+            <v>224.19052099999999</v>
+          </cell>
+          <cell r="S22">
+            <v>224.88494900000001</v>
+          </cell>
+          <cell r="T22">
+            <v>225.54260300000001</v>
+          </cell>
+          <cell r="U22">
+            <v>226.167709</v>
+          </cell>
+          <cell r="V22">
+            <v>226.76289399999999</v>
+          </cell>
+          <cell r="W22">
+            <v>227.33021500000001</v>
+          </cell>
+          <cell r="X22">
+            <v>227.87237500000001</v>
+          </cell>
+          <cell r="Y22">
+            <v>228.39172400000001</v>
+          </cell>
+          <cell r="Z22">
+            <v>228.89146400000001</v>
+          </cell>
+          <cell r="AA22">
+            <v>229.376724</v>
+          </cell>
+          <cell r="AB22">
+            <v>229.852081</v>
+          </cell>
+          <cell r="AC22">
+            <v>230.323227</v>
+          </cell>
+          <cell r="AD22">
+            <v>230.79690600000001</v>
+          </cell>
+          <cell r="AE22">
+            <v>231.280609</v>
+          </cell>
+          <cell r="AF22">
+            <v>231.78066999999999</v>
+          </cell>
+          <cell r="AG22">
+            <v>232.30583200000001</v>
+          </cell>
+          <cell r="AH22">
+            <v>232.850571</v>
+          </cell>
+          <cell r="AI22">
+            <v>3.3159999999999999E-3</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>TKI000:railpassmiles</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v xml:space="preserve">   Passenger Rail</v>
+          </cell>
+          <cell r="C23">
+            <v>41.270718000000002</v>
+          </cell>
+          <cell r="D23">
+            <v>41.874930999999997</v>
+          </cell>
+          <cell r="E23">
+            <v>42.455513000000003</v>
+          </cell>
+          <cell r="F23">
+            <v>42.941440999999998</v>
+          </cell>
+          <cell r="G23">
+            <v>43.403492</v>
+          </cell>
+          <cell r="H23">
+            <v>43.866782999999998</v>
+          </cell>
+          <cell r="I23">
+            <v>44.310471</v>
+          </cell>
+          <cell r="J23">
+            <v>44.751930000000002</v>
+          </cell>
+          <cell r="K23">
+            <v>45.177658000000001</v>
+          </cell>
+          <cell r="L23">
+            <v>45.617381999999999</v>
+          </cell>
+          <cell r="M23">
+            <v>46.05724</v>
+          </cell>
+          <cell r="N23">
+            <v>46.402245000000001</v>
+          </cell>
+          <cell r="O23">
+            <v>46.841445999999998</v>
+          </cell>
+          <cell r="P23">
+            <v>47.267837999999998</v>
+          </cell>
+          <cell r="Q23">
+            <v>47.680484999999997</v>
+          </cell>
+          <cell r="R23">
+            <v>48.055225</v>
+          </cell>
+          <cell r="S23">
+            <v>48.435218999999996</v>
+          </cell>
+          <cell r="T23">
+            <v>48.803921000000003</v>
+          </cell>
+          <cell r="U23">
+            <v>49.166313000000002</v>
+          </cell>
+          <cell r="V23">
+            <v>49.530780999999998</v>
+          </cell>
+          <cell r="W23">
+            <v>49.890510999999996</v>
+          </cell>
+          <cell r="X23">
+            <v>50.244216999999999</v>
+          </cell>
+          <cell r="Y23">
+            <v>50.573273</v>
+          </cell>
+          <cell r="Z23">
+            <v>50.897018000000003</v>
+          </cell>
+          <cell r="AA23">
+            <v>51.222712999999999</v>
+          </cell>
+          <cell r="AB23">
+            <v>51.549354999999998</v>
+          </cell>
+          <cell r="AC23">
+            <v>51.873221999999998</v>
+          </cell>
+          <cell r="AD23">
+            <v>52.227497</v>
+          </cell>
+          <cell r="AE23">
+            <v>52.585467999999999</v>
+          </cell>
+          <cell r="AF23">
+            <v>52.972960999999998</v>
+          </cell>
+          <cell r="AG23">
+            <v>53.355491999999998</v>
+          </cell>
+          <cell r="AH23">
+            <v>53.757781999999999</v>
+          </cell>
+          <cell r="AI23">
+            <v>8.5629999999999994E-3</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>TKI000:da_RecreationalB</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v xml:space="preserve">    Recreational Boats</v>
+          </cell>
+          <cell r="C64">
+            <v>0.24548700000000001</v>
+          </cell>
+          <cell r="D64">
+            <v>0.24624699999999999</v>
+          </cell>
+          <cell r="E64">
+            <v>0.246891</v>
+          </cell>
+          <cell r="F64">
+            <v>0.247228</v>
+          </cell>
+          <cell r="G64">
+            <v>0.24740100000000001</v>
+          </cell>
+          <cell r="H64">
+            <v>0.247561</v>
+          </cell>
+          <cell r="I64">
+            <v>0.247747</v>
+          </cell>
+          <cell r="J64">
+            <v>0.24787200000000001</v>
+          </cell>
+          <cell r="K64">
+            <v>0.247948</v>
+          </cell>
+          <cell r="L64">
+            <v>0.248034</v>
+          </cell>
+          <cell r="M64">
+            <v>0.24811900000000001</v>
+          </cell>
+          <cell r="N64">
+            <v>0.24812799999999999</v>
+          </cell>
+          <cell r="O64">
+            <v>0.24811900000000001</v>
+          </cell>
+          <cell r="P64">
+            <v>0.24807899999999999</v>
+          </cell>
+          <cell r="Q64">
+            <v>0.247943</v>
+          </cell>
+          <cell r="R64">
+            <v>0.24770400000000001</v>
+          </cell>
+          <cell r="S64">
+            <v>0.24738199999999999</v>
+          </cell>
+          <cell r="T64">
+            <v>0.24705099999999999</v>
+          </cell>
+          <cell r="U64">
+            <v>0.246672</v>
+          </cell>
+          <cell r="V64">
+            <v>0.24627099999999999</v>
+          </cell>
+          <cell r="W64">
+            <v>0.24584500000000001</v>
+          </cell>
+          <cell r="X64">
+            <v>0.245364</v>
+          </cell>
+          <cell r="Y64">
+            <v>0.244837</v>
+          </cell>
+          <cell r="Z64">
+            <v>0.24424299999999999</v>
+          </cell>
+          <cell r="AA64">
+            <v>0.24363599999999999</v>
+          </cell>
+          <cell r="AB64">
+            <v>0.243037</v>
+          </cell>
+          <cell r="AC64">
+            <v>0.24246699999999999</v>
+          </cell>
+          <cell r="AD64">
+            <v>0.241926</v>
+          </cell>
+          <cell r="AE64">
+            <v>0.24138699999999999</v>
+          </cell>
+          <cell r="AF64">
+            <v>0.24085799999999999</v>
+          </cell>
+          <cell r="AG64">
+            <v>0.240316</v>
+          </cell>
+          <cell r="AH64">
+            <v>0.23976</v>
+          </cell>
+          <cell r="AI64">
+            <v>-7.6099999999999996E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="E1">
+            <v>2019</v>
+          </cell>
+          <cell r="F1">
+            <v>2020</v>
+          </cell>
+          <cell r="G1">
+            <v>2021</v>
+          </cell>
+          <cell r="H1">
+            <v>2022</v>
+          </cell>
+          <cell r="I1">
+            <v>2023</v>
+          </cell>
+          <cell r="J1">
+            <v>2024</v>
+          </cell>
+          <cell r="K1">
+            <v>2025</v>
+          </cell>
+          <cell r="L1">
+            <v>2026</v>
+          </cell>
+          <cell r="M1">
+            <v>2027</v>
+          </cell>
+          <cell r="N1">
+            <v>2028</v>
+          </cell>
+          <cell r="O1">
+            <v>2029</v>
+          </cell>
+          <cell r="P1">
+            <v>2030</v>
+          </cell>
+          <cell r="Q1">
+            <v>2031</v>
+          </cell>
+          <cell r="R1">
+            <v>2032</v>
+          </cell>
+          <cell r="S1">
+            <v>2033</v>
+          </cell>
+          <cell r="T1">
+            <v>2034</v>
+          </cell>
+          <cell r="U1">
+            <v>2035</v>
+          </cell>
+          <cell r="V1">
+            <v>2036</v>
+          </cell>
+          <cell r="W1">
+            <v>2037</v>
+          </cell>
+          <cell r="X1">
+            <v>2038</v>
+          </cell>
+          <cell r="Y1">
+            <v>2039</v>
+          </cell>
+          <cell r="Z1">
+            <v>2040</v>
+          </cell>
+          <cell r="AA1">
+            <v>2041</v>
+          </cell>
+          <cell r="AB1">
+            <v>2042</v>
+          </cell>
+          <cell r="AC1">
+            <v>2043</v>
+          </cell>
+          <cell r="AD1">
+            <v>2044</v>
+          </cell>
+          <cell r="AE1">
+            <v>2045</v>
+          </cell>
+          <cell r="AF1">
+            <v>2046</v>
+          </cell>
+          <cell r="AG1">
+            <v>2047</v>
+          </cell>
+          <cell r="AH1">
+            <v>2048</v>
+          </cell>
+          <cell r="AI1">
+            <v>2049</v>
+          </cell>
+          <cell r="AJ1">
+            <v>2050</v>
+          </cell>
+          <cell r="AK1" t="str">
+            <v>Growth (2019-2050)</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Motorcycles</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Transportation Energy Use: Highway: Light-Duty Vehicles: Motorcycles: High oil and gas supply</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>45-AEO2020.7.highogs-d112619a</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>trillion Btu</v>
+          </cell>
+          <cell r="E12">
+            <v>18.970794999999999</v>
+          </cell>
+          <cell r="F12">
+            <v>18.823608</v>
+          </cell>
+          <cell r="G12">
+            <v>18.561443000000001</v>
+          </cell>
+          <cell r="H12">
+            <v>18.168322</v>
+          </cell>
+          <cell r="I12">
+            <v>17.638919999999999</v>
+          </cell>
+          <cell r="J12">
+            <v>17.075298</v>
+          </cell>
+          <cell r="K12">
+            <v>16.499818999999999</v>
+          </cell>
+          <cell r="L12">
+            <v>16.021494000000001</v>
+          </cell>
+          <cell r="M12">
+            <v>15.598401000000001</v>
+          </cell>
+          <cell r="N12">
+            <v>15.213685999999999</v>
+          </cell>
+          <cell r="O12">
+            <v>14.869465999999999</v>
+          </cell>
+          <cell r="P12">
+            <v>14.583327000000001</v>
+          </cell>
+          <cell r="Q12">
+            <v>14.346128999999999</v>
+          </cell>
+          <cell r="R12">
+            <v>14.126972</v>
+          </cell>
+          <cell r="S12">
+            <v>13.94516</v>
+          </cell>
+          <cell r="T12">
+            <v>13.787245</v>
+          </cell>
+          <cell r="U12">
+            <v>13.654823</v>
+          </cell>
+          <cell r="V12">
+            <v>13.585337000000001</v>
+          </cell>
+          <cell r="W12">
+            <v>13.553765</v>
+          </cell>
+          <cell r="X12">
+            <v>13.559089999999999</v>
+          </cell>
+          <cell r="Y12">
+            <v>13.600536999999999</v>
+          </cell>
+          <cell r="Z12">
+            <v>13.677015000000001</v>
+          </cell>
+          <cell r="AA12">
+            <v>13.769792000000001</v>
+          </cell>
+          <cell r="AB12">
+            <v>13.886583999999999</v>
+          </cell>
+          <cell r="AC12">
+            <v>14.020749</v>
+          </cell>
+          <cell r="AD12">
+            <v>14.167451</v>
+          </cell>
+          <cell r="AE12">
+            <v>14.327847999999999</v>
+          </cell>
+          <cell r="AF12">
+            <v>14.508926000000001</v>
+          </cell>
+          <cell r="AG12">
+            <v>14.702455</v>
+          </cell>
+          <cell r="AH12">
+            <v>14.911671999999999</v>
+          </cell>
+          <cell r="AI12">
+            <v>15.129991</v>
+          </cell>
+          <cell r="AJ12">
+            <v>15.353588999999999</v>
+          </cell>
+          <cell r="AK12">
+            <v>-7.0000000000000001E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="E1">
+            <v>2019</v>
+          </cell>
+          <cell r="F1">
+            <v>2020</v>
+          </cell>
+          <cell r="G1">
+            <v>2021</v>
+          </cell>
+          <cell r="H1">
+            <v>2022</v>
+          </cell>
+          <cell r="I1">
+            <v>2023</v>
+          </cell>
+          <cell r="J1">
+            <v>2024</v>
+          </cell>
+          <cell r="K1">
+            <v>2025</v>
+          </cell>
+          <cell r="L1">
+            <v>2026</v>
+          </cell>
+          <cell r="M1">
+            <v>2027</v>
+          </cell>
+          <cell r="N1">
+            <v>2028</v>
+          </cell>
+          <cell r="O1">
+            <v>2029</v>
+          </cell>
+          <cell r="P1">
+            <v>2030</v>
+          </cell>
+          <cell r="Q1">
+            <v>2031</v>
+          </cell>
+          <cell r="R1">
+            <v>2032</v>
+          </cell>
+          <cell r="S1">
+            <v>2033</v>
+          </cell>
+          <cell r="T1">
+            <v>2034</v>
+          </cell>
+          <cell r="U1">
+            <v>2035</v>
+          </cell>
+          <cell r="V1">
+            <v>2036</v>
+          </cell>
+          <cell r="W1">
+            <v>2037</v>
+          </cell>
+          <cell r="X1">
+            <v>2038</v>
+          </cell>
+          <cell r="Y1">
+            <v>2039</v>
+          </cell>
+          <cell r="Z1">
+            <v>2040</v>
+          </cell>
+          <cell r="AA1">
+            <v>2041</v>
+          </cell>
+          <cell r="AB1">
+            <v>2042</v>
+          </cell>
+          <cell r="AC1">
+            <v>2043</v>
+          </cell>
+          <cell r="AD1">
+            <v>2044</v>
+          </cell>
+          <cell r="AE1">
+            <v>2045</v>
+          </cell>
+          <cell r="AF1">
+            <v>2046</v>
+          </cell>
+          <cell r="AG1">
+            <v>2047</v>
+          </cell>
+          <cell r="AH1">
+            <v>2048</v>
+          </cell>
+          <cell r="AI1">
+            <v>2049</v>
+          </cell>
+          <cell r="AJ1">
+            <v>2050</v>
+          </cell>
+          <cell r="AK1" t="str">
+            <v>Growth (2019-2050)</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>United States</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Air Travel: Travel Demand: Revenue Passenger Miles: Domestic: U.S.: High oil and gas supply</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>57-AEO2020.47.highogs-d112619a</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>billion miles</v>
+          </cell>
+          <cell r="E41">
+            <v>721.91784700000005</v>
+          </cell>
+          <cell r="F41">
+            <v>734.06219499999997</v>
+          </cell>
+          <cell r="G41">
+            <v>747.42523200000005</v>
+          </cell>
+          <cell r="H41">
+            <v>757.89398200000005</v>
+          </cell>
+          <cell r="I41">
+            <v>766.14849900000002</v>
+          </cell>
+          <cell r="J41">
+            <v>775.42034899999999</v>
+          </cell>
+          <cell r="K41">
+            <v>785.53460700000005</v>
+          </cell>
+          <cell r="L41">
+            <v>795.18792699999995</v>
+          </cell>
+          <cell r="M41">
+            <v>805.01843299999996</v>
+          </cell>
+          <cell r="N41">
+            <v>815.72650099999998</v>
+          </cell>
+          <cell r="O41">
+            <v>827.55218500000001</v>
+          </cell>
+          <cell r="P41">
+            <v>839.68627900000001</v>
+          </cell>
+          <cell r="Q41">
+            <v>851.99041699999998</v>
+          </cell>
+          <cell r="R41">
+            <v>864.56347700000003</v>
+          </cell>
+          <cell r="S41">
+            <v>876.85357699999997</v>
+          </cell>
+          <cell r="T41">
+            <v>887.97845500000005</v>
+          </cell>
+          <cell r="U41">
+            <v>898.65393100000006</v>
+          </cell>
+          <cell r="V41">
+            <v>910.13421600000004</v>
+          </cell>
+          <cell r="W41">
+            <v>921.73034700000005</v>
+          </cell>
+          <cell r="X41">
+            <v>933.70996100000002</v>
+          </cell>
+          <cell r="Y41">
+            <v>946.13281199999994</v>
+          </cell>
+          <cell r="Z41">
+            <v>958.79187000000002</v>
+          </cell>
+          <cell r="AA41">
+            <v>970.88244599999996</v>
+          </cell>
+          <cell r="AB41">
+            <v>982.95562700000005</v>
+          </cell>
+          <cell r="AC41">
+            <v>995.20153800000003</v>
+          </cell>
+          <cell r="AD41">
+            <v>1008.019592</v>
+          </cell>
+          <cell r="AE41">
+            <v>1022.330383</v>
+          </cell>
+          <cell r="AF41">
+            <v>1037.8583980000001</v>
+          </cell>
+          <cell r="AG41">
+            <v>1054.029663</v>
+          </cell>
+          <cell r="AH41">
+            <v>1071.330078</v>
+          </cell>
+          <cell r="AI41">
+            <v>1089.0820309999999</v>
+          </cell>
+          <cell r="AJ41">
+            <v>1107.07251</v>
+          </cell>
+          <cell r="AK41">
+            <v>1.4E-2</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>United States</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>Air Travel: Travel Demand: Revenue Passenger Miles: International: U.S.: High oil and gas supply</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>57-AEO2020.61.highogs-d112619a</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>billion miles</v>
+          </cell>
+          <cell r="E55">
+            <v>297.88812300000001</v>
+          </cell>
+          <cell r="F55">
+            <v>306.09170499999999</v>
+          </cell>
+          <cell r="G55">
+            <v>314.998627</v>
+          </cell>
+          <cell r="H55">
+            <v>322.75979599999999</v>
+          </cell>
+          <cell r="I55">
+            <v>329.65463299999999</v>
+          </cell>
+          <cell r="J55">
+            <v>337.15154999999999</v>
+          </cell>
+          <cell r="K55">
+            <v>345.18383799999998</v>
+          </cell>
+          <cell r="L55">
+            <v>353.15145899999999</v>
+          </cell>
+          <cell r="M55">
+            <v>361.35427900000002</v>
+          </cell>
+          <cell r="N55">
+            <v>370.13232399999998</v>
+          </cell>
+          <cell r="O55">
+            <v>379.61450200000002</v>
+          </cell>
+          <cell r="P55">
+            <v>389.42440800000003</v>
+          </cell>
+          <cell r="Q55">
+            <v>399.50158699999997</v>
+          </cell>
+          <cell r="R55">
+            <v>409.899475</v>
+          </cell>
+          <cell r="S55">
+            <v>420.34811400000001</v>
+          </cell>
+          <cell r="T55">
+            <v>430.40139799999997</v>
+          </cell>
+          <cell r="U55">
+            <v>440.41061400000001</v>
+          </cell>
+          <cell r="V55">
+            <v>451.01641799999999</v>
+          </cell>
+          <cell r="W55">
+            <v>461.87530500000003</v>
+          </cell>
+          <cell r="X55">
+            <v>473.13122600000003</v>
+          </cell>
+          <cell r="Y55">
+            <v>484.82379200000003</v>
+          </cell>
+          <cell r="Z55">
+            <v>496.85177599999997</v>
+          </cell>
+          <cell r="AA55">
+            <v>508.78909299999998</v>
+          </cell>
+          <cell r="AB55">
+            <v>520.92913799999997</v>
+          </cell>
+          <cell r="AC55">
+            <v>533.37811299999998</v>
+          </cell>
+          <cell r="AD55">
+            <v>546.36181599999998</v>
+          </cell>
+          <cell r="AE55">
+            <v>560.40362500000003</v>
+          </cell>
+          <cell r="AF55">
+            <v>575.37377900000001</v>
+          </cell>
+          <cell r="AG55">
+            <v>590.96923800000002</v>
+          </cell>
+          <cell r="AH55">
+            <v>607.48107900000002</v>
+          </cell>
+          <cell r="AI55">
+            <v>624.53930700000001</v>
+          </cell>
+          <cell r="AJ55">
+            <v>642.03161599999999</v>
+          </cell>
+          <cell r="AK55">
+            <v>2.5000000000000001E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>highogs.d120120a</v>
+          </cell>
+          <cell r="C1">
+            <v>2020</v>
+          </cell>
+          <cell r="D1">
+            <v>2021</v>
+          </cell>
+          <cell r="E1">
+            <v>2022</v>
+          </cell>
+          <cell r="F1">
+            <v>2023</v>
+          </cell>
+          <cell r="G1">
+            <v>2024</v>
+          </cell>
+          <cell r="H1">
+            <v>2025</v>
+          </cell>
+          <cell r="I1">
+            <v>2026</v>
+          </cell>
+          <cell r="J1">
+            <v>2027</v>
+          </cell>
+          <cell r="K1">
+            <v>2028</v>
+          </cell>
+          <cell r="L1">
+            <v>2029</v>
+          </cell>
+          <cell r="M1">
+            <v>2030</v>
+          </cell>
+          <cell r="N1">
+            <v>2031</v>
+          </cell>
+          <cell r="O1">
+            <v>2032</v>
+          </cell>
+          <cell r="P1">
+            <v>2033</v>
+          </cell>
+          <cell r="Q1">
+            <v>2034</v>
+          </cell>
+          <cell r="R1">
+            <v>2035</v>
+          </cell>
+          <cell r="S1">
+            <v>2036</v>
+          </cell>
+          <cell r="T1">
+            <v>2037</v>
+          </cell>
+          <cell r="U1">
+            <v>2038</v>
+          </cell>
+          <cell r="V1">
+            <v>2039</v>
+          </cell>
+          <cell r="W1">
+            <v>2040</v>
+          </cell>
+          <cell r="X1">
+            <v>2041</v>
+          </cell>
+          <cell r="Y1">
+            <v>2042</v>
+          </cell>
+          <cell r="Z1">
+            <v>2043</v>
+          </cell>
+          <cell r="AA1">
+            <v>2044</v>
+          </cell>
+          <cell r="AB1">
+            <v>2045</v>
+          </cell>
+          <cell r="AC1">
+            <v>2046</v>
+          </cell>
+          <cell r="AD1">
+            <v>2047</v>
+          </cell>
+          <cell r="AE1">
+            <v>2048</v>
+          </cell>
+          <cell r="AF1">
+            <v>2049</v>
+          </cell>
+          <cell r="AG1">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>TKI000:ba_Light-DutyVeh</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v xml:space="preserve">   Light-Duty Vehicles less than 8,501 pounds</v>
+          </cell>
+          <cell r="C18">
+            <v>2628.821289</v>
+          </cell>
+          <cell r="D18">
+            <v>2807.2766109999998</v>
+          </cell>
+          <cell r="E18">
+            <v>2862.5334469999998</v>
+          </cell>
+          <cell r="F18">
+            <v>2927.623047</v>
+          </cell>
+          <cell r="G18">
+            <v>2985.178711</v>
+          </cell>
+          <cell r="H18">
+            <v>3035.5583499999998</v>
+          </cell>
+          <cell r="I18">
+            <v>3076.6459960000002</v>
+          </cell>
+          <cell r="J18">
+            <v>3107.342529</v>
+          </cell>
+          <cell r="K18">
+            <v>3133.9348140000002</v>
+          </cell>
+          <cell r="L18">
+            <v>3153.696289</v>
+          </cell>
+          <cell r="M18">
+            <v>3170.140625</v>
+          </cell>
+          <cell r="N18">
+            <v>3182.3603520000001</v>
+          </cell>
+          <cell r="O18">
+            <v>3194.3308109999998</v>
+          </cell>
+          <cell r="P18">
+            <v>3208.3691410000001</v>
+          </cell>
+          <cell r="Q18">
+            <v>3223.0124510000001</v>
+          </cell>
+          <cell r="R18">
+            <v>3240.584961</v>
+          </cell>
+          <cell r="S18">
+            <v>3258.4960940000001</v>
+          </cell>
+          <cell r="T18">
+            <v>3274.8767090000001</v>
+          </cell>
+          <cell r="U18">
+            <v>3290.0166020000001</v>
+          </cell>
+          <cell r="V18">
+            <v>3306.976807</v>
+          </cell>
+          <cell r="W18">
+            <v>3326.3066410000001</v>
+          </cell>
+          <cell r="X18">
+            <v>3344.3862300000001</v>
+          </cell>
+          <cell r="Y18">
+            <v>3362.8256839999999</v>
+          </cell>
+          <cell r="Z18">
+            <v>3380.6958009999998</v>
+          </cell>
+          <cell r="AA18">
+            <v>3396.751953</v>
+          </cell>
+          <cell r="AB18">
+            <v>3412.030518</v>
+          </cell>
+          <cell r="AC18">
+            <v>3428.1083979999999</v>
+          </cell>
+          <cell r="AD18">
+            <v>3442.514893</v>
+          </cell>
+          <cell r="AE18">
+            <v>3458.3400879999999</v>
+          </cell>
+          <cell r="AF18">
+            <v>3474.70874</v>
+          </cell>
+          <cell r="AG18">
+            <v>3490.9399410000001</v>
+          </cell>
+          <cell r="AH18">
+            <v>9.4990000000000005E-3</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>TKI000:buspassmiles</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v xml:space="preserve">   Bus Transportation</v>
+          </cell>
+          <cell r="C22">
+            <v>108.32250999999999</v>
+          </cell>
+          <cell r="D22">
+            <v>134.82925399999999</v>
+          </cell>
+          <cell r="E22">
+            <v>154.717422</v>
+          </cell>
+          <cell r="F22">
+            <v>169.65283199999999</v>
+          </cell>
+          <cell r="G22">
+            <v>180.920807</v>
+          </cell>
+          <cell r="H22">
+            <v>189.44929500000001</v>
+          </cell>
+          <cell r="I22">
+            <v>195.917755</v>
+          </cell>
+          <cell r="J22">
+            <v>200.87158199999999</v>
+          </cell>
+          <cell r="K22">
+            <v>204.42939799999999</v>
+          </cell>
+          <cell r="L22">
+            <v>207.178192</v>
+          </cell>
+          <cell r="M22">
+            <v>209.42626999999999</v>
+          </cell>
+          <cell r="N22">
+            <v>211.01544200000001</v>
+          </cell>
+          <cell r="O22">
+            <v>212.35484299999999</v>
+          </cell>
+          <cell r="P22">
+            <v>213.36850000000001</v>
+          </cell>
+          <cell r="Q22">
+            <v>214.16456600000001</v>
+          </cell>
+          <cell r="R22">
+            <v>214.70815999999999</v>
+          </cell>
+          <cell r="S22">
+            <v>215.16941800000001</v>
+          </cell>
+          <cell r="T22">
+            <v>215.53512599999999</v>
+          </cell>
+          <cell r="U22">
+            <v>215.80548099999999</v>
+          </cell>
+          <cell r="V22">
+            <v>215.98587000000001</v>
+          </cell>
+          <cell r="W22">
+            <v>216.16197199999999</v>
+          </cell>
+          <cell r="X22">
+            <v>216.26544200000001</v>
+          </cell>
+          <cell r="Y22">
+            <v>216.33122299999999</v>
+          </cell>
+          <cell r="Z22">
+            <v>216.37844799999999</v>
+          </cell>
+          <cell r="AA22">
+            <v>216.409988</v>
+          </cell>
+          <cell r="AB22">
+            <v>216.441574</v>
+          </cell>
+          <cell r="AC22">
+            <v>216.45150799999999</v>
+          </cell>
+          <cell r="AD22">
+            <v>216.468369</v>
+          </cell>
+          <cell r="AE22">
+            <v>216.483002</v>
+          </cell>
+          <cell r="AF22">
+            <v>216.552536</v>
+          </cell>
+          <cell r="AG22">
+            <v>216.64347799999999</v>
+          </cell>
+          <cell r="AH22">
+            <v>2.3373999999999999E-2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>TKI000:railpassmiles</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v xml:space="preserve">   Passenger Rail</v>
+          </cell>
+          <cell r="C23">
+            <v>24.970692</v>
+          </cell>
+          <cell r="D23">
+            <v>29.653244000000001</v>
+          </cell>
+          <cell r="E23">
+            <v>33.486446000000001</v>
+          </cell>
+          <cell r="F23">
+            <v>36.386100999999996</v>
+          </cell>
+          <cell r="G23">
+            <v>38.577961000000002</v>
+          </cell>
+          <cell r="H23">
+            <v>40.222988000000001</v>
+          </cell>
+          <cell r="I23">
+            <v>41.396163999999999</v>
+          </cell>
+          <cell r="J23">
+            <v>42.264778</v>
+          </cell>
+          <cell r="K23">
+            <v>42.515728000000003</v>
+          </cell>
+          <cell r="L23">
+            <v>42.713290999999998</v>
+          </cell>
+          <cell r="M23">
+            <v>43.137005000000002</v>
+          </cell>
+          <cell r="N23">
+            <v>43.343741999999999</v>
+          </cell>
+          <cell r="O23">
+            <v>43.818241</v>
+          </cell>
+          <cell r="P23">
+            <v>44.274138999999998</v>
+          </cell>
+          <cell r="Q23">
+            <v>44.835864999999998</v>
+          </cell>
+          <cell r="R23">
+            <v>45.310886000000004</v>
+          </cell>
+          <cell r="S23">
+            <v>45.831733999999997</v>
+          </cell>
+          <cell r="T23">
+            <v>46.327930000000002</v>
+          </cell>
+          <cell r="U23">
+            <v>46.816153999999997</v>
+          </cell>
+          <cell r="V23">
+            <v>47.317447999999999</v>
+          </cell>
+          <cell r="W23">
+            <v>47.980491999999998</v>
+          </cell>
+          <cell r="X23">
+            <v>48.582149999999999</v>
+          </cell>
+          <cell r="Y23">
+            <v>49.164020999999998</v>
+          </cell>
+          <cell r="Z23">
+            <v>49.763081</v>
+          </cell>
+          <cell r="AA23">
+            <v>50.334721000000002</v>
+          </cell>
+          <cell r="AB23">
+            <v>50.978020000000001</v>
+          </cell>
+          <cell r="AC23">
+            <v>51.558666000000002</v>
+          </cell>
+          <cell r="AD23">
+            <v>52.079247000000002</v>
+          </cell>
+          <cell r="AE23">
+            <v>52.647174999999997</v>
+          </cell>
+          <cell r="AF23">
+            <v>53.282265000000002</v>
+          </cell>
+          <cell r="AG23">
+            <v>53.912506</v>
+          </cell>
+          <cell r="AH23">
+            <v>2.5987E-2</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>TKI000:da_RecreationalB</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v xml:space="preserve">    Recreational Boats</v>
+          </cell>
+          <cell r="C64">
+            <v>0.195878</v>
+          </cell>
+          <cell r="D64">
+            <v>0.196657</v>
+          </cell>
+          <cell r="E64">
+            <v>0.199716</v>
+          </cell>
+          <cell r="F64">
+            <v>0.201514</v>
+          </cell>
+          <cell r="G64">
+            <v>0.20225699999999999</v>
+          </cell>
+          <cell r="H64">
+            <v>0.202574</v>
+          </cell>
+          <cell r="I64">
+            <v>0.20185400000000001</v>
+          </cell>
+          <cell r="J64">
+            <v>0.200378</v>
+          </cell>
+          <cell r="K64">
+            <v>0.19867399999999999</v>
+          </cell>
+          <cell r="L64">
+            <v>0.19683</v>
+          </cell>
+          <cell r="M64">
+            <v>0.19506899999999999</v>
+          </cell>
+          <cell r="N64">
+            <v>0.19355600000000001</v>
+          </cell>
+          <cell r="O64">
+            <v>0.19248899999999999</v>
+          </cell>
+          <cell r="P64">
+            <v>0.191383</v>
+          </cell>
+          <cell r="Q64">
+            <v>0.19048399999999999</v>
+          </cell>
+          <cell r="R64">
+            <v>0.18981799999999999</v>
+          </cell>
+          <cell r="S64">
+            <v>0.18890999999999999</v>
+          </cell>
+          <cell r="T64">
+            <v>0.18775900000000001</v>
+          </cell>
+          <cell r="U64">
+            <v>0.18665799999999999</v>
+          </cell>
+          <cell r="V64">
+            <v>0.18580199999999999</v>
+          </cell>
+          <cell r="W64">
+            <v>0.185223</v>
+          </cell>
+          <cell r="X64">
+            <v>0.184588</v>
+          </cell>
+          <cell r="Y64">
+            <v>0.18388199999999999</v>
+          </cell>
+          <cell r="Z64">
+            <v>0.183175</v>
+          </cell>
+          <cell r="AA64">
+            <v>0.18232899999999999</v>
+          </cell>
+          <cell r="AB64">
+            <v>0.18168000000000001</v>
+          </cell>
+          <cell r="AC64">
+            <v>0.18090600000000001</v>
+          </cell>
+          <cell r="AD64">
+            <v>0.17988000000000001</v>
+          </cell>
+          <cell r="AE64">
+            <v>0.17913999999999999</v>
+          </cell>
+          <cell r="AF64">
+            <v>0.178366</v>
+          </cell>
+          <cell r="AG64">
+            <v>0.17757200000000001</v>
+          </cell>
+          <cell r="AH64">
+            <v>-3.2650000000000001E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="E1">
+            <v>2020</v>
+          </cell>
+          <cell r="F1">
+            <v>2021</v>
+          </cell>
+          <cell r="G1">
+            <v>2022</v>
+          </cell>
+          <cell r="H1">
+            <v>2023</v>
+          </cell>
+          <cell r="I1">
+            <v>2024</v>
+          </cell>
+          <cell r="J1">
+            <v>2025</v>
+          </cell>
+          <cell r="K1">
+            <v>2026</v>
+          </cell>
+          <cell r="L1">
+            <v>2027</v>
+          </cell>
+          <cell r="M1">
+            <v>2028</v>
+          </cell>
+          <cell r="N1">
+            <v>2029</v>
+          </cell>
+          <cell r="O1">
+            <v>2030</v>
+          </cell>
+          <cell r="P1">
+            <v>2031</v>
+          </cell>
+          <cell r="Q1">
+            <v>2032</v>
+          </cell>
+          <cell r="R1">
+            <v>2033</v>
+          </cell>
+          <cell r="S1">
+            <v>2034</v>
+          </cell>
+          <cell r="T1">
+            <v>2035</v>
+          </cell>
+          <cell r="U1">
+            <v>2036</v>
+          </cell>
+          <cell r="V1">
+            <v>2037</v>
+          </cell>
+          <cell r="W1">
+            <v>2038</v>
+          </cell>
+          <cell r="X1">
+            <v>2039</v>
+          </cell>
+          <cell r="Y1">
+            <v>2040</v>
+          </cell>
+          <cell r="Z1">
+            <v>2041</v>
+          </cell>
+          <cell r="AA1">
+            <v>2042</v>
+          </cell>
+          <cell r="AB1">
+            <v>2043</v>
+          </cell>
+          <cell r="AC1">
+            <v>2044</v>
+          </cell>
+          <cell r="AD1">
+            <v>2045</v>
+          </cell>
+          <cell r="AE1">
+            <v>2046</v>
+          </cell>
+          <cell r="AF1">
+            <v>2047</v>
+          </cell>
+          <cell r="AG1">
+            <v>2048</v>
+          </cell>
+          <cell r="AH1">
+            <v>2049</v>
+          </cell>
+          <cell r="AI1">
+            <v>2050</v>
+          </cell>
+          <cell r="AJ1" t="str">
+            <v>Growth (2020-2050)</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Motorcycles</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>Transportation Energy Use: Highway: Light-Duty Vehicles: Motorcycles: High oil and gas supply</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>45-AEO2021.7.highogs-d120120a</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>trillion Btu</v>
+          </cell>
+          <cell r="E20">
+            <v>16.299149</v>
+          </cell>
+          <cell r="F20">
+            <v>16.800868999999999</v>
+          </cell>
+          <cell r="G20">
+            <v>16.528765</v>
+          </cell>
+          <cell r="H20">
+            <v>16.295639000000001</v>
+          </cell>
+          <cell r="I20">
+            <v>15.999691</v>
+          </cell>
+          <cell r="J20">
+            <v>15.658419</v>
+          </cell>
+          <cell r="K20">
+            <v>15.284882</v>
+          </cell>
+          <cell r="L20">
+            <v>14.892150000000001</v>
+          </cell>
+          <cell r="M20">
+            <v>14.502713999999999</v>
+          </cell>
+          <cell r="N20">
+            <v>14.107929</v>
+          </cell>
+          <cell r="O20">
+            <v>13.741054</v>
+          </cell>
+          <cell r="P20">
+            <v>13.388216</v>
+          </cell>
+          <cell r="Q20">
+            <v>13.066401000000001</v>
+          </cell>
+          <cell r="R20">
+            <v>12.787572000000001</v>
+          </cell>
+          <cell r="S20">
+            <v>12.547905999999999</v>
+          </cell>
+          <cell r="T20">
+            <v>12.350932999999999</v>
+          </cell>
+          <cell r="U20">
+            <v>12.189022</v>
+          </cell>
+          <cell r="V20">
+            <v>12.054244000000001</v>
+          </cell>
+          <cell r="W20">
+            <v>11.942542</v>
+          </cell>
+          <cell r="X20">
+            <v>11.857060000000001</v>
+          </cell>
+          <cell r="Y20">
+            <v>11.799364000000001</v>
+          </cell>
+          <cell r="Z20">
+            <v>11.751442000000001</v>
+          </cell>
+          <cell r="AA20">
+            <v>11.71702</v>
+          </cell>
+          <cell r="AB20">
+            <v>11.690611000000001</v>
+          </cell>
+          <cell r="AC20">
+            <v>11.666224</v>
+          </cell>
+          <cell r="AD20">
+            <v>11.642757</v>
+          </cell>
+          <cell r="AE20">
+            <v>11.624537</v>
+          </cell>
+          <cell r="AF20">
+            <v>11.602817999999999</v>
+          </cell>
+          <cell r="AG20">
+            <v>11.586204</v>
+          </cell>
+          <cell r="AH20">
+            <v>11.573715</v>
+          </cell>
+          <cell r="AI20">
+            <v>11.561806000000001</v>
+          </cell>
+          <cell r="AJ20">
+            <v>-1.0999999999999999E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="E1">
+            <v>2020</v>
+          </cell>
+          <cell r="F1">
+            <v>2021</v>
+          </cell>
+          <cell r="G1">
+            <v>2022</v>
+          </cell>
+          <cell r="H1">
+            <v>2023</v>
+          </cell>
+          <cell r="I1">
+            <v>2024</v>
+          </cell>
+          <cell r="J1">
+            <v>2025</v>
+          </cell>
+          <cell r="K1">
+            <v>2026</v>
+          </cell>
+          <cell r="L1">
+            <v>2027</v>
+          </cell>
+          <cell r="M1">
+            <v>2028</v>
+          </cell>
+          <cell r="N1">
+            <v>2029</v>
+          </cell>
+          <cell r="O1">
+            <v>2030</v>
+          </cell>
+          <cell r="P1">
+            <v>2031</v>
+          </cell>
+          <cell r="Q1">
+            <v>2032</v>
+          </cell>
+          <cell r="R1">
+            <v>2033</v>
+          </cell>
+          <cell r="S1">
+            <v>2034</v>
+          </cell>
+          <cell r="T1">
+            <v>2035</v>
+          </cell>
+          <cell r="U1">
+            <v>2036</v>
+          </cell>
+          <cell r="V1">
+            <v>2037</v>
+          </cell>
+          <cell r="W1">
+            <v>2038</v>
+          </cell>
+          <cell r="X1">
+            <v>2039</v>
+          </cell>
+          <cell r="Y1">
+            <v>2040</v>
+          </cell>
+          <cell r="Z1">
+            <v>2041</v>
+          </cell>
+          <cell r="AA1">
+            <v>2042</v>
+          </cell>
+          <cell r="AB1">
+            <v>2043</v>
+          </cell>
+          <cell r="AC1">
+            <v>2044</v>
+          </cell>
+          <cell r="AD1">
+            <v>2045</v>
+          </cell>
+          <cell r="AE1">
+            <v>2046</v>
+          </cell>
+          <cell r="AF1">
+            <v>2047</v>
+          </cell>
+          <cell r="AG1">
+            <v>2048</v>
+          </cell>
+          <cell r="AH1">
+            <v>2049</v>
+          </cell>
+          <cell r="AI1">
+            <v>2050</v>
+          </cell>
+          <cell r="AJ1" t="str">
+            <v>Growth (2020-2050)</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>United States</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Air Travel: Travel Demand: Revenue Passenger Miles: Domestic: U.S.: High oil and gas supply</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>57-AEO2021.47.highogs-d120120a</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>billion miles</v>
+          </cell>
+          <cell r="E41">
+            <v>369.825378</v>
+          </cell>
+          <cell r="F41">
+            <v>580.62579300000004</v>
+          </cell>
+          <cell r="G41">
+            <v>676.04077099999995</v>
+          </cell>
+          <cell r="H41">
+            <v>724.85772699999995</v>
+          </cell>
+          <cell r="I41">
+            <v>752.83508300000005</v>
+          </cell>
+          <cell r="J41">
+            <v>778.23168899999996</v>
+          </cell>
+          <cell r="K41">
+            <v>796.84307899999999</v>
+          </cell>
+          <cell r="L41">
+            <v>809.83221400000002</v>
+          </cell>
+          <cell r="M41">
+            <v>820.70532200000002</v>
+          </cell>
+          <cell r="N41">
+            <v>830.52337599999998</v>
+          </cell>
+          <cell r="O41">
+            <v>840.79162599999995</v>
+          </cell>
+          <cell r="P41">
+            <v>852.89044200000001</v>
+          </cell>
+          <cell r="Q41">
+            <v>868.67492700000003</v>
+          </cell>
+          <cell r="R41">
+            <v>884.73956299999998</v>
+          </cell>
+          <cell r="S41">
+            <v>903.00506600000006</v>
+          </cell>
+          <cell r="T41">
+            <v>923.197632</v>
+          </cell>
+          <cell r="U41">
+            <v>941.32788100000005</v>
+          </cell>
+          <cell r="V41">
+            <v>957.51031499999999</v>
+          </cell>
+          <cell r="W41">
+            <v>974.28094499999997</v>
+          </cell>
+          <cell r="X41">
+            <v>993.48870799999997</v>
+          </cell>
+          <cell r="Y41">
+            <v>1015.347839</v>
+          </cell>
+          <cell r="Z41">
+            <v>1036.888672</v>
+          </cell>
+          <cell r="AA41">
+            <v>1058.3245850000001</v>
+          </cell>
+          <cell r="AB41">
+            <v>1079.478638</v>
+          </cell>
+          <cell r="AC41">
+            <v>1099.933716</v>
+          </cell>
+          <cell r="AD41">
+            <v>1122.0977780000001</v>
+          </cell>
+          <cell r="AE41">
+            <v>1142.5672609999999</v>
+          </cell>
+          <cell r="AF41">
+            <v>1161.0610349999999</v>
+          </cell>
+          <cell r="AG41">
+            <v>1182.670044</v>
+          </cell>
+          <cell r="AH41">
+            <v>1204.3160399999999</v>
+          </cell>
+          <cell r="AI41">
+            <v>1226.4289550000001</v>
+          </cell>
+          <cell r="AJ41">
+            <v>4.1000000000000002E-2</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>United States</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>Air Travel: Travel Demand: Revenue Passenger Miles: International: U.S.: High oil and gas supply</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>57-AEO2021.61.highogs-d120120a</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>billion miles</v>
+          </cell>
+          <cell r="E55">
+            <v>65.570098999999999</v>
+          </cell>
+          <cell r="F55">
+            <v>203.26728800000001</v>
+          </cell>
+          <cell r="G55">
+            <v>285.88558999999998</v>
+          </cell>
+          <cell r="H55">
+            <v>335.45660400000003</v>
+          </cell>
+          <cell r="I55">
+            <v>372.63482699999997</v>
+          </cell>
+          <cell r="J55">
+            <v>394.94174199999998</v>
+          </cell>
+          <cell r="K55">
+            <v>405.67648300000002</v>
+          </cell>
+          <cell r="L55">
+            <v>414.17031900000001</v>
+          </cell>
+          <cell r="M55">
+            <v>421.857574</v>
+          </cell>
+          <cell r="N55">
+            <v>429.17263800000001</v>
+          </cell>
+          <cell r="O55">
+            <v>436.74331699999999</v>
+          </cell>
+          <cell r="P55">
+            <v>445.15548699999999</v>
+          </cell>
+          <cell r="Q55">
+            <v>455.21203600000001</v>
+          </cell>
+          <cell r="R55">
+            <v>465.47653200000002</v>
+          </cell>
+          <cell r="S55">
+            <v>476.77606200000002</v>
+          </cell>
+          <cell r="T55">
+            <v>489.003784</v>
+          </cell>
+          <cell r="U55">
+            <v>500.44461100000001</v>
+          </cell>
+          <cell r="V55">
+            <v>511.139679</v>
+          </cell>
+          <cell r="W55">
+            <v>522.18554700000004</v>
+          </cell>
+          <cell r="X55">
+            <v>534.39581299999998</v>
+          </cell>
+          <cell r="Y55">
+            <v>547.87725799999998</v>
+          </cell>
+          <cell r="Z55">
+            <v>561.33587599999998</v>
+          </cell>
+          <cell r="AA55">
+            <v>574.86657700000001</v>
+          </cell>
+          <cell r="AB55">
+            <v>588.392517</v>
+          </cell>
+          <cell r="AC55">
+            <v>601.72943099999998</v>
+          </cell>
+          <cell r="AD55">
+            <v>615.95178199999998</v>
+          </cell>
+          <cell r="AE55">
+            <v>629.54540999999995</v>
+          </cell>
+          <cell r="AF55">
+            <v>642.37738000000002</v>
+          </cell>
+          <cell r="AG55">
+            <v>656.73962400000005</v>
+          </cell>
+          <cell r="AH55">
+            <v>671.25531000000001</v>
+          </cell>
+          <cell r="AI55">
+            <v>686.12292500000001</v>
+          </cell>
+          <cell r="AJ55">
+            <v>8.1000000000000003E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>ref2022.d011222a</v>
+          </cell>
+          <cell r="C1">
+            <v>2021</v>
+          </cell>
+          <cell r="D1">
+            <v>2022</v>
+          </cell>
+          <cell r="E1">
+            <v>2023</v>
+          </cell>
+          <cell r="F1">
+            <v>2024</v>
+          </cell>
+          <cell r="G1">
+            <v>2025</v>
+          </cell>
+          <cell r="H1">
+            <v>2026</v>
+          </cell>
+          <cell r="I1">
+            <v>2027</v>
+          </cell>
+          <cell r="J1">
+            <v>2028</v>
+          </cell>
+          <cell r="K1">
+            <v>2029</v>
+          </cell>
+          <cell r="L1">
+            <v>2030</v>
+          </cell>
+          <cell r="M1">
+            <v>2031</v>
+          </cell>
+          <cell r="N1">
+            <v>2032</v>
+          </cell>
+          <cell r="O1">
+            <v>2033</v>
+          </cell>
+          <cell r="P1">
+            <v>2034</v>
+          </cell>
+          <cell r="Q1">
+            <v>2035</v>
+          </cell>
+          <cell r="R1">
+            <v>2036</v>
+          </cell>
+          <cell r="S1">
+            <v>2037</v>
+          </cell>
+          <cell r="T1">
+            <v>2038</v>
+          </cell>
+          <cell r="U1">
+            <v>2039</v>
+          </cell>
+          <cell r="V1">
+            <v>2040</v>
+          </cell>
+          <cell r="W1">
+            <v>2041</v>
+          </cell>
+          <cell r="X1">
+            <v>2042</v>
+          </cell>
+          <cell r="Y1">
+            <v>2043</v>
+          </cell>
+          <cell r="Z1">
+            <v>2044</v>
+          </cell>
+          <cell r="AA1">
+            <v>2045</v>
+          </cell>
+          <cell r="AB1">
+            <v>2046</v>
+          </cell>
+          <cell r="AC1">
+            <v>2047</v>
+          </cell>
+          <cell r="AD1">
+            <v>2048</v>
+          </cell>
+          <cell r="AE1">
+            <v>2049</v>
+          </cell>
+          <cell r="AF1">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>TKI000:ba_Light-DutyVeh</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v xml:space="preserve">   Light-Duty Vehicles less than 8,501 pounds</v>
+          </cell>
+          <cell r="C18">
+            <v>2747.6179200000001</v>
+          </cell>
+          <cell r="D18">
+            <v>2846.6770019999999</v>
+          </cell>
+          <cell r="E18">
+            <v>2931.8728030000002</v>
+          </cell>
+          <cell r="F18">
+            <v>2967.975586</v>
+          </cell>
+          <cell r="G18">
+            <v>2996.234375</v>
+          </cell>
+          <cell r="H18">
+            <v>3018.3295899999998</v>
+          </cell>
+          <cell r="I18">
+            <v>3033.9277339999999</v>
+          </cell>
+          <cell r="J18">
+            <v>3047.1857909999999</v>
+          </cell>
+          <cell r="K18">
+            <v>3059.5039059999999</v>
+          </cell>
+          <cell r="L18">
+            <v>3073.7705080000001</v>
+          </cell>
+          <cell r="M18">
+            <v>3089.7641600000002</v>
+          </cell>
+          <cell r="N18">
+            <v>3099.4091800000001</v>
+          </cell>
+          <cell r="O18">
+            <v>3109.859375</v>
+          </cell>
+          <cell r="P18">
+            <v>3116.404297</v>
+          </cell>
+          <cell r="Q18">
+            <v>3120.2697750000002</v>
+          </cell>
+          <cell r="R18">
+            <v>3124.3608399999998</v>
+          </cell>
+          <cell r="S18">
+            <v>3130.0383299999999</v>
+          </cell>
+          <cell r="T18">
+            <v>3137.4807129999999</v>
+          </cell>
+          <cell r="U18">
+            <v>3149.3427729999999</v>
+          </cell>
+          <cell r="V18">
+            <v>3162.850586</v>
+          </cell>
+          <cell r="W18">
+            <v>3176.188232</v>
+          </cell>
+          <cell r="X18">
+            <v>3191.0429690000001</v>
+          </cell>
+          <cell r="Y18">
+            <v>3205.969971</v>
+          </cell>
+          <cell r="Z18">
+            <v>3221.5429690000001</v>
+          </cell>
+          <cell r="AA18">
+            <v>3239.27124</v>
+          </cell>
+          <cell r="AB18">
+            <v>3260.9125979999999</v>
+          </cell>
+          <cell r="AC18">
+            <v>3285.2683109999998</v>
+          </cell>
+          <cell r="AD18">
+            <v>3310.0817870000001</v>
+          </cell>
+          <cell r="AE18">
+            <v>3336.3100589999999</v>
+          </cell>
+          <cell r="AF18">
+            <v>3367.272461</v>
+          </cell>
+          <cell r="AG18">
+            <v>7.0369999999999999E-3</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>TKI000:buspassmiles</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v xml:space="preserve">   Bus Transportation</v>
+          </cell>
+          <cell r="C22">
+            <v>151.12510700000001</v>
+          </cell>
+          <cell r="D22">
+            <v>172.57624799999999</v>
+          </cell>
+          <cell r="E22">
+            <v>183.98443599999999</v>
+          </cell>
+          <cell r="F22">
+            <v>190.58796699999999</v>
+          </cell>
+          <cell r="G22">
+            <v>194.82553100000001</v>
+          </cell>
+          <cell r="H22">
+            <v>197.64862099999999</v>
+          </cell>
+          <cell r="I22">
+            <v>199.61532600000001</v>
+          </cell>
+          <cell r="J22">
+            <v>201.019012</v>
+          </cell>
+          <cell r="K22">
+            <v>202.00473</v>
+          </cell>
+          <cell r="L22">
+            <v>202.72674599999999</v>
+          </cell>
+          <cell r="M22">
+            <v>203.187378</v>
+          </cell>
+          <cell r="N22">
+            <v>203.61854600000001</v>
+          </cell>
+          <cell r="O22">
+            <v>203.85322600000001</v>
+          </cell>
+          <cell r="P22">
+            <v>203.99607800000001</v>
+          </cell>
+          <cell r="Q22">
+            <v>204.043228</v>
+          </cell>
+          <cell r="R22">
+            <v>204.07839999999999</v>
+          </cell>
+          <cell r="S22">
+            <v>204.18630999999999</v>
+          </cell>
+          <cell r="T22">
+            <v>204.21899400000001</v>
+          </cell>
+          <cell r="U22">
+            <v>203.99002100000001</v>
+          </cell>
+          <cell r="V22">
+            <v>203.792114</v>
+          </cell>
+          <cell r="W22">
+            <v>203.48487900000001</v>
+          </cell>
+          <cell r="X22">
+            <v>203.15222199999999</v>
+          </cell>
+          <cell r="Y22">
+            <v>202.79278600000001</v>
+          </cell>
+          <cell r="Z22">
+            <v>202.389938</v>
+          </cell>
+          <cell r="AA22">
+            <v>201.98461900000001</v>
+          </cell>
+          <cell r="AB22">
+            <v>201.58862300000001</v>
+          </cell>
+          <cell r="AC22">
+            <v>201.169388</v>
+          </cell>
+          <cell r="AD22">
+            <v>200.720001</v>
+          </cell>
+          <cell r="AE22">
+            <v>200.25181599999999</v>
+          </cell>
+          <cell r="AF22">
+            <v>199.751251</v>
+          </cell>
+          <cell r="AG22">
+            <v>9.6659999999999992E-3</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>TKI000:railpassmiles</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v xml:space="preserve">   Passenger Rail</v>
+          </cell>
+          <cell r="C23">
+            <v>29.302727000000001</v>
+          </cell>
+          <cell r="D23">
+            <v>32.183658999999999</v>
+          </cell>
+          <cell r="E23">
+            <v>34.523235</v>
+          </cell>
+          <cell r="F23">
+            <v>36.408005000000003</v>
+          </cell>
+          <cell r="G23">
+            <v>37.782608000000003</v>
+          </cell>
+          <cell r="H23">
+            <v>38.852116000000002</v>
+          </cell>
+          <cell r="I23">
+            <v>39.682259000000002</v>
+          </cell>
+          <cell r="J23">
+            <v>40.435603999999998</v>
+          </cell>
+          <cell r="K23">
+            <v>41.089024000000002</v>
+          </cell>
+          <cell r="L23">
+            <v>41.799472999999999</v>
+          </cell>
+          <cell r="M23">
+            <v>42.392325999999997</v>
+          </cell>
+          <cell r="N23">
+            <v>43.226954999999997</v>
+          </cell>
+          <cell r="O23">
+            <v>43.855072</v>
+          </cell>
+          <cell r="P23">
+            <v>44.286602000000002</v>
+          </cell>
+          <cell r="Q23">
+            <v>44.641052000000002</v>
+          </cell>
+          <cell r="R23">
+            <v>44.98415</v>
+          </cell>
+          <cell r="S23">
+            <v>45.384822999999997</v>
+          </cell>
+          <cell r="T23">
+            <v>45.809635</v>
+          </cell>
+          <cell r="U23">
+            <v>46.217002999999998</v>
+          </cell>
+          <cell r="V23">
+            <v>46.775120000000001</v>
+          </cell>
+          <cell r="W23">
+            <v>47.199725999999998</v>
+          </cell>
+          <cell r="X23">
+            <v>47.657195999999999</v>
+          </cell>
+          <cell r="Y23">
+            <v>48.122261000000002</v>
+          </cell>
+          <cell r="Z23">
+            <v>48.558163</v>
+          </cell>
+          <cell r="AA23">
+            <v>49.064247000000002</v>
+          </cell>
+          <cell r="AB23">
+            <v>49.669609000000001</v>
+          </cell>
+          <cell r="AC23">
+            <v>50.250259</v>
+          </cell>
+          <cell r="AD23">
+            <v>50.763556999999999</v>
+          </cell>
+          <cell r="AE23">
+            <v>51.312564999999999</v>
+          </cell>
+          <cell r="AF23">
+            <v>51.905762000000003</v>
+          </cell>
+          <cell r="AG23">
+            <v>1.9911000000000002E-2</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>TKI000:da_RecreationalB</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v xml:space="preserve">    Recreational Boats</v>
+          </cell>
+          <cell r="C64">
+            <v>0.20260800000000001</v>
+          </cell>
+          <cell r="D64">
+            <v>0.20266999999999999</v>
+          </cell>
+          <cell r="E64">
+            <v>0.20230200000000001</v>
+          </cell>
+          <cell r="F64">
+            <v>0.20225799999999999</v>
+          </cell>
+          <cell r="G64">
+            <v>0.20154</v>
+          </cell>
+          <cell r="H64">
+            <v>0.20046600000000001</v>
+          </cell>
+          <cell r="I64">
+            <v>0.198825</v>
+          </cell>
+          <cell r="J64">
+            <v>0.197571</v>
+          </cell>
+          <cell r="K64">
+            <v>0.19638700000000001</v>
+          </cell>
+          <cell r="L64">
+            <v>0.195377</v>
+          </cell>
+          <cell r="M64">
+            <v>0.194215</v>
+          </cell>
+          <cell r="N64">
+            <v>0.19345499999999999</v>
+          </cell>
+          <cell r="O64">
+            <v>0.19265399999999999</v>
+          </cell>
+          <cell r="P64">
+            <v>0.191359</v>
+          </cell>
+          <cell r="Q64">
+            <v>0.19001499999999999</v>
+          </cell>
+          <cell r="R64">
+            <v>0.18870799999999999</v>
+          </cell>
+          <cell r="S64">
+            <v>0.18769</v>
+          </cell>
+          <cell r="T64">
+            <v>0.18674299999999999</v>
+          </cell>
+          <cell r="U64">
+            <v>0.18589700000000001</v>
+          </cell>
+          <cell r="V64">
+            <v>0.18516199999999999</v>
+          </cell>
+          <cell r="W64">
+            <v>0.184172</v>
+          </cell>
+          <cell r="X64">
+            <v>0.183249</v>
+          </cell>
+          <cell r="Y64">
+            <v>0.18237500000000001</v>
+          </cell>
+          <cell r="Z64">
+            <v>0.181536</v>
+          </cell>
+          <cell r="AA64">
+            <v>0.180867</v>
+          </cell>
+          <cell r="AB64">
+            <v>0.18041699999999999</v>
+          </cell>
+          <cell r="AC64">
+            <v>0.17985400000000001</v>
+          </cell>
+          <cell r="AD64">
+            <v>0.179121</v>
+          </cell>
+          <cell r="AE64">
+            <v>0.178563</v>
+          </cell>
+          <cell r="AF64">
+            <v>0.178365</v>
+          </cell>
+          <cell r="AG64">
+            <v>-4.385E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13">
+        <row r="13">
+          <cell r="B13" t="str">
+            <v xml:space="preserve"> Mode and Type</v>
+          </cell>
+          <cell r="C13">
+            <v>2021</v>
+          </cell>
+          <cell r="D13">
+            <v>2022</v>
+          </cell>
+          <cell r="E13">
+            <v>2023</v>
+          </cell>
+          <cell r="F13">
+            <v>2024</v>
+          </cell>
+          <cell r="G13">
+            <v>2025</v>
+          </cell>
+          <cell r="H13">
+            <v>2026</v>
+          </cell>
+          <cell r="I13">
+            <v>2027</v>
+          </cell>
+          <cell r="J13">
+            <v>2028</v>
+          </cell>
+          <cell r="K13">
+            <v>2029</v>
+          </cell>
+          <cell r="L13">
+            <v>2030</v>
+          </cell>
+          <cell r="M13">
+            <v>2031</v>
+          </cell>
+          <cell r="N13">
+            <v>2032</v>
+          </cell>
+          <cell r="O13">
+            <v>2033</v>
+          </cell>
+          <cell r="P13">
+            <v>2034</v>
+          </cell>
+          <cell r="Q13">
+            <v>2035</v>
+          </cell>
+          <cell r="R13">
+            <v>2036</v>
+          </cell>
+          <cell r="S13">
+            <v>2037</v>
+          </cell>
+          <cell r="T13">
+            <v>2038</v>
+          </cell>
+          <cell r="U13">
+            <v>2039</v>
+          </cell>
+          <cell r="V13">
+            <v>2040</v>
+          </cell>
+          <cell r="W13">
+            <v>2041</v>
+          </cell>
+          <cell r="X13">
+            <v>2042</v>
+          </cell>
+          <cell r="Y13">
+            <v>2043</v>
+          </cell>
+          <cell r="Z13">
+            <v>2044</v>
+          </cell>
+          <cell r="AA13">
+            <v>2045</v>
+          </cell>
+          <cell r="AB13">
+            <v>2046</v>
+          </cell>
+          <cell r="AC13">
+            <v>2047</v>
+          </cell>
+          <cell r="AD13">
+            <v>2048</v>
+          </cell>
+          <cell r="AE13">
+            <v>2049</v>
+          </cell>
+          <cell r="AF13">
+            <v>2050</v>
+          </cell>
+          <cell r="AG13" t="str">
+            <v>2021–2050</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>TEU000:ba_Motorcycles</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v xml:space="preserve">         Motorcycles</v>
+          </cell>
+          <cell r="C20">
+            <v>16.196756000000001</v>
+          </cell>
+          <cell r="D20">
+            <v>16.068059999999999</v>
+          </cell>
+          <cell r="E20">
+            <v>15.797902000000001</v>
+          </cell>
+          <cell r="F20">
+            <v>15.217829999999999</v>
+          </cell>
+          <cell r="G20">
+            <v>14.582477000000001</v>
+          </cell>
+          <cell r="H20">
+            <v>13.902256</v>
+          </cell>
+          <cell r="I20">
+            <v>13.205594</v>
+          </cell>
+          <cell r="J20">
+            <v>12.522964</v>
+          </cell>
+          <cell r="K20">
+            <v>11.857192</v>
+          </cell>
+          <cell r="L20">
+            <v>11.236345</v>
+          </cell>
+          <cell r="M20">
+            <v>10.662895000000001</v>
+          </cell>
+          <cell r="N20">
+            <v>10.118478</v>
+          </cell>
+          <cell r="O20">
+            <v>9.6304219999999994</v>
+          </cell>
+          <cell r="P20">
+            <v>9.1882950000000001</v>
+          </cell>
+          <cell r="Q20">
+            <v>8.7799049999999994</v>
+          </cell>
+          <cell r="R20">
+            <v>8.4229590000000005</v>
+          </cell>
+          <cell r="S20">
+            <v>8.1219649999999994</v>
+          </cell>
+          <cell r="T20">
+            <v>7.8791960000000003</v>
+          </cell>
+          <cell r="U20">
+            <v>7.682385</v>
+          </cell>
+          <cell r="V20">
+            <v>7.5297689999999999</v>
+          </cell>
+          <cell r="W20">
+            <v>7.4058089999999996</v>
+          </cell>
+          <cell r="X20">
+            <v>7.3144590000000003</v>
+          </cell>
+          <cell r="Y20">
+            <v>7.247967</v>
+          </cell>
+          <cell r="Z20">
+            <v>7.200075</v>
+          </cell>
+          <cell r="AA20">
+            <v>7.1688049999999999</v>
+          </cell>
+          <cell r="AB20">
+            <v>7.1552119999999997</v>
+          </cell>
+          <cell r="AC20">
+            <v>7.1522129999999997</v>
+          </cell>
+          <cell r="AD20">
+            <v>7.1525920000000003</v>
+          </cell>
+          <cell r="AE20">
+            <v>7.1573669999999998</v>
+          </cell>
+          <cell r="AF20">
+            <v>7.1712860000000003</v>
+          </cell>
+          <cell r="AG20">
+            <v>-2.8000000000000001E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17">
+        <row r="13">
+          <cell r="B13" t="str">
+            <v xml:space="preserve"> Indicators</v>
+          </cell>
+          <cell r="C13">
+            <v>2021</v>
+          </cell>
+          <cell r="D13">
+            <v>2022</v>
+          </cell>
+          <cell r="E13">
+            <v>2023</v>
+          </cell>
+          <cell r="F13">
+            <v>2024</v>
+          </cell>
+          <cell r="G13">
+            <v>2025</v>
+          </cell>
+          <cell r="H13">
+            <v>2026</v>
+          </cell>
+          <cell r="I13">
+            <v>2027</v>
+          </cell>
+          <cell r="J13">
+            <v>2028</v>
+          </cell>
+          <cell r="K13">
+            <v>2029</v>
+          </cell>
+          <cell r="L13">
+            <v>2030</v>
+          </cell>
+          <cell r="M13">
+            <v>2031</v>
+          </cell>
+          <cell r="N13">
+            <v>2032</v>
+          </cell>
+          <cell r="O13">
+            <v>2033</v>
+          </cell>
+          <cell r="P13">
+            <v>2034</v>
+          </cell>
+          <cell r="Q13">
+            <v>2035</v>
+          </cell>
+          <cell r="R13">
+            <v>2036</v>
+          </cell>
+          <cell r="S13">
+            <v>2037</v>
+          </cell>
+          <cell r="T13">
+            <v>2038</v>
+          </cell>
+          <cell r="U13">
+            <v>2039</v>
+          </cell>
+          <cell r="V13">
+            <v>2040</v>
+          </cell>
+          <cell r="W13">
+            <v>2041</v>
+          </cell>
+          <cell r="X13">
+            <v>2042</v>
+          </cell>
+          <cell r="Y13">
+            <v>2043</v>
+          </cell>
+          <cell r="Z13">
+            <v>2044</v>
+          </cell>
+          <cell r="AA13">
+            <v>2045</v>
+          </cell>
+          <cell r="AB13">
+            <v>2046</v>
+          </cell>
+          <cell r="AC13">
+            <v>2047</v>
+          </cell>
+          <cell r="AD13">
+            <v>2048</v>
+          </cell>
+          <cell r="AE13">
+            <v>2049</v>
+          </cell>
+          <cell r="AF13">
+            <v>2050</v>
+          </cell>
+          <cell r="AG13" t="str">
+            <v>2021–2050</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>ATE000:rpm_US_Domestic</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v xml:space="preserve">      United States</v>
+          </cell>
+          <cell r="C45">
+            <v>535.94671600000004</v>
+          </cell>
+          <cell r="D45">
+            <v>667.29132100000004</v>
+          </cell>
+          <cell r="E45">
+            <v>719.82916299999999</v>
+          </cell>
+          <cell r="F45">
+            <v>742.01489300000003</v>
+          </cell>
+          <cell r="G45">
+            <v>759.67718500000001</v>
+          </cell>
+          <cell r="H45">
+            <v>775.02557400000001</v>
+          </cell>
+          <cell r="I45">
+            <v>786.07965100000001</v>
+          </cell>
+          <cell r="J45">
+            <v>799.764771</v>
+          </cell>
+          <cell r="K45">
+            <v>814.21252400000003</v>
+          </cell>
+          <cell r="L45">
+            <v>830.07330300000001</v>
+          </cell>
+          <cell r="M45">
+            <v>844.87103300000001</v>
+          </cell>
+          <cell r="N45">
+            <v>862.62341300000003</v>
+          </cell>
+          <cell r="O45">
+            <v>879.68713400000001</v>
+          </cell>
+          <cell r="P45">
+            <v>892.413635</v>
+          </cell>
+          <cell r="Q45">
+            <v>903.95611599999995</v>
+          </cell>
+          <cell r="R45">
+            <v>915.12323000000004</v>
+          </cell>
+          <cell r="S45">
+            <v>928.09375</v>
+          </cell>
+          <cell r="T45">
+            <v>941.50689699999998</v>
+          </cell>
+          <cell r="U45">
+            <v>957.27099599999997</v>
+          </cell>
+          <cell r="V45">
+            <v>974.25744599999996</v>
+          </cell>
+          <cell r="W45">
+            <v>988.66180399999996</v>
+          </cell>
+          <cell r="X45">
+            <v>1004.493835</v>
+          </cell>
+          <cell r="Y45">
+            <v>1021.2597050000001</v>
+          </cell>
+          <cell r="Z45">
+            <v>1037.251953</v>
+          </cell>
+          <cell r="AA45">
+            <v>1055.8355710000001</v>
+          </cell>
+          <cell r="AB45">
+            <v>1075.9636230000001</v>
+          </cell>
+          <cell r="AC45">
+            <v>1095.3867190000001</v>
+          </cell>
+          <cell r="AD45">
+            <v>1114.5532229999999</v>
+          </cell>
+          <cell r="AE45">
+            <v>1135.255737</v>
+          </cell>
+          <cell r="AF45">
+            <v>1160.4592290000001</v>
+          </cell>
+          <cell r="AG45">
+            <v>2.7E-2</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>ATE000:rpm_US_Internat</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v xml:space="preserve">      United States</v>
+          </cell>
+          <cell r="C59">
+            <v>94.195380999999998</v>
+          </cell>
+          <cell r="D59">
+            <v>188.800308</v>
+          </cell>
+          <cell r="E59">
+            <v>299.172729</v>
+          </cell>
+          <cell r="F59">
+            <v>354.35891700000002</v>
+          </cell>
+          <cell r="G59">
+            <v>381.95202599999999</v>
+          </cell>
+          <cell r="H59">
+            <v>390.98666400000002</v>
+          </cell>
+          <cell r="I59">
+            <v>398.33737200000002</v>
+          </cell>
+          <cell r="J59">
+            <v>406.84954800000003</v>
+          </cell>
+          <cell r="K59">
+            <v>415.75982699999997</v>
+          </cell>
+          <cell r="L59">
+            <v>425.34075899999999</v>
+          </cell>
+          <cell r="M59">
+            <v>434.560608</v>
+          </cell>
+          <cell r="N59">
+            <v>445.09667999999999</v>
+          </cell>
+          <cell r="O59">
+            <v>455.425568</v>
+          </cell>
+          <cell r="P59">
+            <v>464.004456</v>
+          </cell>
+          <cell r="Q59">
+            <v>472.14825400000001</v>
+          </cell>
+          <cell r="R59">
+            <v>480.19339000000002</v>
+          </cell>
+          <cell r="S59">
+            <v>489.07055700000001</v>
+          </cell>
+          <cell r="T59">
+            <v>498.20519999999999</v>
+          </cell>
+          <cell r="U59">
+            <v>508.42764299999999</v>
+          </cell>
+          <cell r="V59">
+            <v>519.26086399999997</v>
+          </cell>
+          <cell r="W59">
+            <v>529.05749500000002</v>
+          </cell>
+          <cell r="X59">
+            <v>539.55963099999997</v>
+          </cell>
+          <cell r="Y59">
+            <v>550.55847200000005</v>
+          </cell>
+          <cell r="Z59">
+            <v>561.30755599999998</v>
+          </cell>
+          <cell r="AA59">
+            <v>573.29119900000001</v>
+          </cell>
+          <cell r="AB59">
+            <v>586.05957000000001</v>
+          </cell>
+          <cell r="AC59">
+            <v>598.62298599999997</v>
+          </cell>
+          <cell r="AD59">
+            <v>611.17883300000005</v>
+          </cell>
+          <cell r="AE59">
+            <v>624.52874799999995</v>
+          </cell>
+          <cell r="AF59">
+            <v>640.01232900000002</v>
+          </cell>
+          <cell r="AG59">
+            <v>6.8000000000000005E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20">
+        <row r="9">
+          <cell r="N9">
+            <v>0.73062991639276853</v>
+          </cell>
+          <cell r="O9">
+            <v>0.78745839193649592</v>
+          </cell>
+          <cell r="P9">
+            <v>0.86400049885466279</v>
+          </cell>
+          <cell r="Q9">
+            <v>0.90260342223031664</v>
+          </cell>
+          <cell r="R9">
+            <v>0.93597010512066947</v>
+          </cell>
+          <cell r="S9">
+            <v>0.94898294693875407</v>
+          </cell>
+          <cell r="T9">
+            <v>0.95429629861976351</v>
+          </cell>
+          <cell r="U9">
+            <v>0.95692971782745007</v>
+          </cell>
+          <cell r="V9">
+            <v>0.9575791122357209</v>
+          </cell>
+          <cell r="W9">
+            <v>0.96113691576263016</v>
+          </cell>
+          <cell r="X9">
+            <v>0.96601012890628035</v>
+          </cell>
+          <cell r="Y9">
+            <v>0.97216953914699133</v>
+          </cell>
+          <cell r="Z9">
+            <v>0.97763116481680834</v>
+          </cell>
+          <cell r="AA9">
+            <v>0.98829192602418225</v>
+          </cell>
+          <cell r="AB9">
+            <v>1.0037708112855954</v>
+          </cell>
+          <cell r="AC9">
+            <v>1.0144891936031093</v>
+          </cell>
+          <cell r="AD9">
+            <v>1.0237582275724348</v>
+          </cell>
+          <cell r="AE9">
+            <v>1.0318409646795581</v>
+          </cell>
+          <cell r="AF9">
+            <v>1.0391242138788364</v>
+          </cell>
+          <cell r="AG9">
+            <v>1.0450381554748394</v>
+          </cell>
+          <cell r="AH9">
+            <v>1.0511862819164084</v>
+          </cell>
+          <cell r="AI9">
+            <v>1.0567129284709647</v>
+          </cell>
+          <cell r="AJ9">
+            <v>1.0617603247045067</v>
+          </cell>
+          <cell r="AK9">
+            <v>1.0671763294626997</v>
+          </cell>
+          <cell r="AL9">
+            <v>1.0764020428396395</v>
+          </cell>
+          <cell r="AM9">
+            <v>1.0837358570798108</v>
+          </cell>
+          <cell r="AN9">
+            <v>1.0902436624725804</v>
+          </cell>
+          <cell r="AO9">
+            <v>1.0949683712903693</v>
+          </cell>
+          <cell r="AP9">
+            <v>1.0998867247813013</v>
+          </cell>
+          <cell r="AQ9">
+            <v>1.1062901756583892</v>
+          </cell>
+          <cell r="AR9">
+            <v>1.1102704497502462</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1872,10 +5149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1983,40 +5260,40 @@
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="14"/>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2062,76 +5339,86 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>110</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2313,19 +5600,19 @@
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:3" s="11" customFormat="1">
-      <c r="A22" s="20" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <v>2009</v>
       </c>
     </row>
@@ -2355,10 +5642,10 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="11">
         <v>2009</v>
       </c>
     </row>
@@ -2458,7 +5745,7 @@
       <c r="A40" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="6">
         <v>2967</v>
       </c>
     </row>
@@ -2466,7 +5753,7 @@
       <c r="A41" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="6">
         <v>100</v>
       </c>
     </row>
@@ -2474,7 +5761,7 @@
       <c r="A42" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="6">
         <v>27876</v>
       </c>
       <c r="C42" t="s">
@@ -2485,7 +5772,7 @@
       <c r="A43" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="6">
         <v>4151</v>
       </c>
       <c r="C43" t="s">
@@ -2493,7 +5780,7 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="B44" s="15"/>
+      <c r="B44" s="6"/>
       <c r="C44" t="s">
         <v>104</v>
       </c>
@@ -2502,7 +5789,7 @@
       <c r="A45" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="6">
         <v>6614973</v>
       </c>
     </row>
@@ -2510,7 +5797,7 @@
       <c r="A46" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="6">
         <v>5727512</v>
       </c>
     </row>
@@ -2518,7 +5805,7 @@
       <c r="A47" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="6">
         <v>44777151</v>
       </c>
     </row>
@@ -2526,18 +5813,18 @@
       <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="6">
         <v>12172542</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="B49" s="15"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="6">
         <f>B45/B40</f>
         <v>2229.5156723963601</v>
       </c>
@@ -2546,7 +5833,7 @@
       <c r="A51" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="6">
         <f>B46/B41</f>
         <v>57275.12</v>
       </c>
@@ -2555,7 +5842,7 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="6">
         <f t="shared" ref="B52:B53" si="1">B47/B42</f>
         <v>1606.2975678002583</v>
       </c>
@@ -2564,19 +5851,19 @@
       <c r="A53" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="6">
         <f t="shared" si="1"/>
         <v>2932.4360395085523</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="B54" s="15"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="6">
         <f>SUMPRODUCT(B40:B43,B50:B53)/SUM(B40:B43)</f>
         <v>1974.4736422180429</v>
       </c>
@@ -2588,7 +5875,7 @@
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="12">
         <v>2007</v>
       </c>
     </row>
@@ -2601,10 +5888,10 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="11" t="s">
+      <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59">
         <v>17287</v>
       </c>
     </row>
@@ -2632,7 +5919,7 @@
       <c r="A63" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63">
         <v>1670994</v>
       </c>
     </row>
@@ -2652,7 +5939,7 @@
         <f>B64/B63</f>
         <v>1.579999688807979</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2672,13 +5959,932 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F3570E-4A47-4AB4-A491-CEB81259EF5B}">
+  <dimension ref="A1:AG7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="72.5">
+      <c r="A1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1">
+        <v>2019</v>
+      </c>
+      <c r="C1">
+        <v>2020</v>
+      </c>
+      <c r="D1">
+        <v>2021</v>
+      </c>
+      <c r="E1">
+        <v>2022</v>
+      </c>
+      <c r="F1">
+        <v>2023</v>
+      </c>
+      <c r="G1">
+        <v>2024</v>
+      </c>
+      <c r="H1">
+        <v>2025</v>
+      </c>
+      <c r="I1">
+        <v>2026</v>
+      </c>
+      <c r="J1">
+        <v>2027</v>
+      </c>
+      <c r="K1">
+        <v>2028</v>
+      </c>
+      <c r="L1">
+        <v>2029</v>
+      </c>
+      <c r="M1">
+        <v>2030</v>
+      </c>
+      <c r="N1">
+        <v>2031</v>
+      </c>
+      <c r="O1">
+        <v>2032</v>
+      </c>
+      <c r="P1">
+        <v>2033</v>
+      </c>
+      <c r="Q1">
+        <v>2034</v>
+      </c>
+      <c r="R1">
+        <v>2035</v>
+      </c>
+      <c r="S1">
+        <v>2036</v>
+      </c>
+      <c r="T1">
+        <v>2037</v>
+      </c>
+      <c r="U1">
+        <v>2038</v>
+      </c>
+      <c r="V1">
+        <v>2039</v>
+      </c>
+      <c r="W1">
+        <v>2040</v>
+      </c>
+      <c r="X1">
+        <v>2041</v>
+      </c>
+      <c r="Y1">
+        <v>2042</v>
+      </c>
+      <c r="Z1">
+        <v>2043</v>
+      </c>
+      <c r="AA1">
+        <v>2044</v>
+      </c>
+      <c r="AB1">
+        <v>2045</v>
+      </c>
+      <c r="AC1">
+        <v>2046</v>
+      </c>
+      <c r="AD1">
+        <v>2047</v>
+      </c>
+      <c r="AE1">
+        <v>2048</v>
+      </c>
+      <c r="AF1">
+        <v>2049</v>
+      </c>
+      <c r="AG1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <f>INDEX('[2]AEO 2020 7'!18:18,MATCH(B$1,'[2]AEO 2020 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>INDEX('[2]AEO 2021 7'!18:18,MATCH(C$1,'[2]AEO 2021 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.9011288744336301</v>
+      </c>
+      <c r="D2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(D$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.94185095578144951</v>
+      </c>
+      <c r="E2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(E$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97580723856058227</v>
+      </c>
+      <c r="F2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(F$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0050113524282107</v>
+      </c>
+      <c r="G2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(G$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0173869598325038</v>
+      </c>
+      <c r="H2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(H$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0270737387820588</v>
+      </c>
+      <c r="I2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(I$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.034647717396213</v>
+      </c>
+      <c r="J2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(J$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0399945768441294</v>
+      </c>
+      <c r="K2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(K$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0445392821200561</v>
+      </c>
+      <c r="L2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(L$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0487617863851963</v>
+      </c>
+      <c r="M2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(M$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0536522089696632</v>
+      </c>
+      <c r="N2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(N$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0591346438864642</v>
+      </c>
+      <c r="O2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(O$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0624408427721999</v>
+      </c>
+      <c r="P2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(P$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0660230461335944</v>
+      </c>
+      <c r="Q2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(Q$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0682665680572014</v>
+      </c>
+      <c r="R2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(R$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0695916082392265</v>
+      </c>
+      <c r="S2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(S$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0709939769792054</v>
+      </c>
+      <c r="T2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(T$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0729401534632121</v>
+      </c>
+      <c r="U2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(U$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0754913144127818</v>
+      </c>
+      <c r="V2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(V$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0795574884128905</v>
+      </c>
+      <c r="W2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(W$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0841878070943785</v>
+      </c>
+      <c r="X2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(X$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0887597945390428</v>
+      </c>
+      <c r="Y2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(Y$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0938518228518193</v>
+      </c>
+      <c r="Z2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(Z$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0989686227526771</v>
+      </c>
+      <c r="AA2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AA$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1043068624489312</v>
+      </c>
+      <c r="AB2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AB$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1103839042618273</v>
+      </c>
+      <c r="AC2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AC$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1178023060593771</v>
+      </c>
+      <c r="AD2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AD$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1261511566767834</v>
+      </c>
+      <c r="AE2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AE$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1346569230414387</v>
+      </c>
+      <c r="AF2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AF$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1436476647569738</v>
+      </c>
+      <c r="AG2">
+        <f>INDEX('[2]AEO 2022 7'!18:18,MATCH(AG$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!18:18,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1542612102957182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <f>INDEX('[2]AEO 2020 7'!22:22,MATCH(B$1,'[2]AEO 2020 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH(B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>INDEX('[2]AEO 2021 7'!22:22,MATCH(C$1,'[2]AEO 2021 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.51548149405308408</v>
+      </c>
+      <c r="D3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(D$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.71916904386071012</v>
+      </c>
+      <c r="E3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(E$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82125000756643807</v>
+      </c>
+      <c r="F3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(F$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.87553890647284693</v>
+      </c>
+      <c r="G3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(G$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.90696356627722052</v>
+      </c>
+      <c r="H3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(H$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.92712914240600097</v>
+      </c>
+      <c r="I3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(I$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.94056356754114889</v>
+      </c>
+      <c r="J3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(J$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.94992265672548992</v>
+      </c>
+      <c r="K3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(K$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95660247014987787</v>
+      </c>
+      <c r="L3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(L$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96129327160338018</v>
+      </c>
+      <c r="M3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(M$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96472917690515192</v>
+      </c>
+      <c r="N3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(N$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96692121687513288</v>
+      </c>
+      <c r="O3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(O$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96897304455922084</v>
+      </c>
+      <c r="P3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(P$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97008983179969721</v>
+      </c>
+      <c r="Q3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(Q$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.9707696310619971</v>
+      </c>
+      <c r="R3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(R$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97099400688604875</v>
+      </c>
+      <c r="S3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(S$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97116138220913562</v>
+      </c>
+      <c r="T3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(T$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97167490066456352</v>
+      </c>
+      <c r="U3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(U$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97183043617746512</v>
+      </c>
+      <c r="V3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(V$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.97074080721541633</v>
+      </c>
+      <c r="W3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(W$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96979901408263569</v>
+      </c>
+      <c r="X3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(X$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96833695456402413</v>
+      </c>
+      <c r="Y3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(Y$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96675391769230445</v>
+      </c>
+      <c r="Z3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(Z$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96504344582180901</v>
+      </c>
+      <c r="AA3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AA$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.9631263863951367</v>
+      </c>
+      <c r="AB3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AB$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96119756805730372</v>
+      </c>
+      <c r="AC3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AC$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95931311569630284</v>
+      </c>
+      <c r="AD3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AD$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95731807436870298</v>
+      </c>
+      <c r="AE3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AE$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95517954672409766</v>
+      </c>
+      <c r="AF3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AF$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95295156379337309</v>
+      </c>
+      <c r="AG3">
+        <f>INDEX('[2]AEO 2022 7'!22:22,MATCH(AG$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!22:22,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.95056949201465712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <f>SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH(B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH(B1,'[2]AEO 2020 47'!1:1,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH(B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH(B1,'[2]AEO 2020 47'!1:1,0)))</f>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>SUM(INDEX('[2]AEO 2021 47'!41:41,MATCH(C$1,'[2]AEO 2021 47'!1:1,0)),INDEX('[2]AEO 2021 47'!55:55,MATCH(C1,'[2]AEO 2021 47'!1:1,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!N9</f>
+        <v>0.58434443483058296</v>
+      </c>
+      <c r="D4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(D1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(D1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!O9</f>
+        <v>0.78468134571861559</v>
+      </c>
+      <c r="E4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(E1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(E1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!P9</f>
+        <v>0.97160268705936637</v>
+      </c>
+      <c r="F4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(F1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(F1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!Q9</f>
+        <v>1.1070327384542122</v>
+      </c>
+      <c r="G4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(G1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(G1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!R9</f>
+        <v>1.1486272758100493</v>
+      </c>
+      <c r="H4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(H1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(H1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!S9</f>
+        <v>1.179638978160392</v>
+      </c>
+      <c r="I4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(I1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(I1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!T9</f>
+        <v>1.1981255214920665</v>
+      </c>
+      <c r="J4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(J1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(J1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!U9</f>
+        <v>1.2136879738727104</v>
+      </c>
+      <c r="K4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(K1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(K1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!V9</f>
+        <v>1.2355953368628565</v>
+      </c>
+      <c r="L4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(L1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(L1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!W9</f>
+        <v>1.2548520968730004</v>
+      </c>
+      <c r="M4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(M1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(M1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!X9</f>
+        <v>1.2743471697460291</v>
+      </c>
+      <c r="N4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(N1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(N1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!Y9</f>
+        <v>1.2904985697468578</v>
+      </c>
+      <c r="O4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(O1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(O1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!Z9</f>
+        <v>1.3116628224577005</v>
+      </c>
+      <c r="P4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(P1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(P1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AA9</f>
+        <v>1.324692661231186</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(Q1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(Q1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AB9</f>
+        <v>1.3250780526742871</v>
+      </c>
+      <c r="R4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(R1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(R1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AC9</f>
+        <v>1.3301064477473827</v>
+      </c>
+      <c r="S4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(S1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(S1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AD9</f>
+        <v>1.3364656846011096</v>
+      </c>
+      <c r="T4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(T1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(T1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AE9</f>
+        <v>1.3467590106415401</v>
+      </c>
+      <c r="U4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(U1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(U1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AF9</f>
+        <v>1.3585969609882078</v>
+      </c>
+      <c r="V4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(V1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(V1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AG9</f>
+        <v>1.3752922233447593</v>
+      </c>
+      <c r="W4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(W1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(W1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AH9</f>
+        <v>1.3931995213453749</v>
+      </c>
+      <c r="X4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(X1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(X1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AI9</f>
+        <v>1.4083703896802926</v>
+      </c>
+      <c r="Y4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(Y1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(Y1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AJ9</f>
+        <v>1.4259959489413661</v>
+      </c>
+      <c r="Z4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(Z1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(Z1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AK9</f>
+        <v>1.4442706074958402</v>
+      </c>
+      <c r="AA4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AA1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AA1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AL9</f>
+        <v>1.4562527043974669</v>
+      </c>
+      <c r="AB4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AB1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AB1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AM9</f>
+        <v>1.4740556752394678</v>
+      </c>
+      <c r="AC4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AC1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AC1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AN9</f>
+        <v>1.4948442976459269</v>
+      </c>
+      <c r="AD4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AD1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AD1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AO9</f>
+        <v>1.5170390829667917</v>
+      </c>
+      <c r="AE4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AE1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AE1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AP9</f>
+        <v>1.538536684782621</v>
+      </c>
+      <c r="AF4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AF1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AF1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AQ9</f>
+        <v>1.5598142325578639</v>
+      </c>
+      <c r="AG4">
+        <f>SUM(INDEX('[2]AEO 2022 47'!45:45,MATCH(AG1,'[2]AEO 2022 47'!13:13,0)),INDEX('[2]AEO 2022 47'!59:59,MATCH(AG1,'[2]AEO 2022 47'!13:13,0)))/SUM(INDEX('[2]AEO 2020 47'!41:41,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)),INDEX('[2]AEO 2020 47'!55:55,MATCH($B$1,'[2]AEO 2020 47'!1:1,0)))/'[2]aircraft calibration'!AR9</f>
+        <v>1.5901567391853617</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>INDEX('[2]AEO 2020 7'!23:23,MATCH(B$1,'[2]AEO 2020 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>INDEX('[2]AEO 2021 7'!23:23,MATCH(C$1,'[2]AEO 2021 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.60504622187576185</v>
+      </c>
+      <c r="D5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(D$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.71001253237222572</v>
+      </c>
+      <c r="E5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(E$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.77981824789188303</v>
+      </c>
+      <c r="F5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(F$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.83650676976349181</v>
+      </c>
+      <c r="G5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(G$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.88217522651289959</v>
+      </c>
+      <c r="H5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(H$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.91548220702145289</v>
+      </c>
+      <c r="I5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(I$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.94139665803730388</v>
+      </c>
+      <c r="J5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(J$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.96151123418788109</v>
+      </c>
+      <c r="K5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(K$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.9797649752543679</v>
+      </c>
+      <c r="L5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(L$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.99559750814124437</v>
+      </c>
+      <c r="M5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(M$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0128118682112581</v>
+      </c>
+      <c r="N5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(N$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0271768472746221</v>
+      </c>
+      <c r="O5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(O$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0474001203468279</v>
+      </c>
+      <c r="P5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(P$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0626195551044204</v>
+      </c>
+      <c r="Q5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(Q$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0730756368231829</v>
+      </c>
+      <c r="R5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(R$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0816640505260897</v>
+      </c>
+      <c r="S5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(S$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0899774023800604</v>
+      </c>
+      <c r="T5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(T$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.0996858111361183</v>
+      </c>
+      <c r="U5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(U$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1099791140052373</v>
+      </c>
+      <c r="V5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(V$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1198497443150854</v>
+      </c>
+      <c r="W5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(W$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1333730612585902</v>
+      </c>
+      <c r="X5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(X$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1436613726952847</v>
+      </c>
+      <c r="Y5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(Y$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1547459872154393</v>
+      </c>
+      <c r="Z5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(Z$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1660146305184222</v>
+      </c>
+      <c r="AA5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AA$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1765766469098018</v>
+      </c>
+      <c r="AB5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AB$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.1888391910215859</v>
+      </c>
+      <c r="AC5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AC$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.2035072663383273</v>
+      </c>
+      <c r="AD5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AD$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.2175765636061868</v>
+      </c>
+      <c r="AE5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AE$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.2300139047738399</v>
+      </c>
+      <c r="AF5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AF$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.2433165083292226</v>
+      </c>
+      <c r="AG5">
+        <f>INDEX('[2]AEO 2022 7'!23:23,MATCH(AG$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!23:23,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1.2576898226001303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f>INDEX('[2]AEO 2020 7'!64:64,MATCH(B$1,'[2]AEO 2020 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>INDEX('[2]AEO 2021 7'!64:64,MATCH(C$1,'[2]AEO 2021 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.79791597925755742</v>
+      </c>
+      <c r="D6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(D$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82533087291791418</v>
+      </c>
+      <c r="E6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(E$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82558343211656826</v>
+      </c>
+      <c r="F6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(F$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82408437106649235</v>
+      </c>
+      <c r="G6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(G$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82390513550615707</v>
+      </c>
+      <c r="H6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(H$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.82098033704432405</v>
+      </c>
+      <c r="I6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(I$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.81660535995796113</v>
+      </c>
+      <c r="J6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(J$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.80992068826455166</v>
+      </c>
+      <c r="K6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(K$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.80481247479499929</v>
+      </c>
+      <c r="L6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(L$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.79998940880779834</v>
+      </c>
+      <c r="M6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(M$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.79587513799101373</v>
+      </c>
+      <c r="N6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(N$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.79114168978398036</v>
+      </c>
+      <c r="O6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(O$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.78804580283273651</v>
+      </c>
+      <c r="P6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(P$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.78478290092754399</v>
+      </c>
+      <c r="Q6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(Q$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.77950767250404296</v>
+      </c>
+      <c r="R6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(R$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.77403284084289592</v>
+      </c>
+      <c r="S6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(S$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.76870872999384887</v>
+      </c>
+      <c r="T6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(T$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.76456187089336702</v>
+      </c>
+      <c r="U6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(U$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.76070423281069866</v>
+      </c>
+      <c r="V6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(V$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.7572580218097088</v>
+      </c>
+      <c r="W6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(W$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.75426397324501904</v>
+      </c>
+      <c r="X6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(X$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.75023117313747778</v>
+      </c>
+      <c r="Y6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(Y$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.74647129990590133</v>
+      </c>
+      <c r="Z6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(Z$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.74291102991197089</v>
+      </c>
+      <c r="AA6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AA$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.7394933336592161</v>
+      </c>
+      <c r="AB6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AB$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.73676813843502909</v>
+      </c>
+      <c r="AC6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AC$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.73493504747705574</v>
+      </c>
+      <c r="AD6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AD$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.73264164701185808</v>
+      </c>
+      <c r="AE6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AE$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.72965574551809254</v>
+      </c>
+      <c r="AF6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AF$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.72738271273020561</v>
+      </c>
+      <c r="AG6">
+        <f>INDEX('[2]AEO 2022 7'!64:64,MATCH(AG$1,'[2]AEO 2022 7'!1:1,0))/INDEX('[2]AEO 2020 7'!64:64,MATCH($B$1,'[2]AEO 2020 7'!1:1,0))</f>
+        <v>0.72657615270869735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>INDEX('[2]AEO 2020 36'!12:12,MATCH(B$1,'[2]AEO 2020 36'!1:1,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH(B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>INDEX('[2]AEO 2021 35'!20:20,MATCH(C$1,'[2]AEO 2021 35'!1:1,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.85917058299349081</v>
+      </c>
+      <c r="D7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(D1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.85377318135586844</v>
+      </c>
+      <c r="E7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(E1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.84698928010133467</v>
+      </c>
+      <c r="F7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(F1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.83274854849256452</v>
+      </c>
+      <c r="G7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(G1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.80217144299962129</v>
+      </c>
+      <c r="H7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(H1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.76868033205777631</v>
+      </c>
+      <c r="I7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(I1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.73282411201006603</v>
+      </c>
+      <c r="J7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(J1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.69610124404380525</v>
+      </c>
+      <c r="K7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(K1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.66011803933361779</v>
+      </c>
+      <c r="L7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(L1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.6250234636977523</v>
+      </c>
+      <c r="M7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(M1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.59229700178616662</v>
+      </c>
+      <c r="N7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(N1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.56206895915537547</v>
+      </c>
+      <c r="O7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(O1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.53337132154978217</v>
+      </c>
+      <c r="P7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(P1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.50764461900516034</v>
+      </c>
+      <c r="Q7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(Q1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.48433895363900148</v>
+      </c>
+      <c r="R7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(R1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.46281165338616542</v>
+      </c>
+      <c r="S7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(S1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.44399610032157327</v>
+      </c>
+      <c r="T7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(T1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.42812992286301127</v>
+      </c>
+      <c r="U7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(U1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.41533293675884436</v>
+      </c>
+      <c r="V7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(V1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.40495851649864967</v>
+      </c>
+      <c r="W7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(W1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.39691372976198414</v>
+      </c>
+      <c r="X7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(X1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.39037947539889606</v>
+      </c>
+      <c r="Y7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(Y1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.38556417904468426</v>
+      </c>
+      <c r="Z7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(Z1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.38205921259493869</v>
+      </c>
+      <c r="AA7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AA1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.37953470057527905</v>
+      </c>
+      <c r="AB7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AB1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.37788637745545195</v>
+      </c>
+      <c r="AC7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AC1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.37716985503243278</v>
+      </c>
+      <c r="AD7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AD1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.37701176993373237</v>
+      </c>
+      <c r="AE7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AE1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.3770317480105605</v>
+      </c>
+      <c r="AF7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AF1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.3772834506935529</v>
+      </c>
+      <c r="AG7">
+        <f>INDEX('[2]AEO 2022 35'!20:20,MATCH(AG1,'[2]AEO 2022 35'!13:13,0))/INDEX('[2]AEO 2020 36'!12:12,MATCH($B$1,'[2]AEO 2020 36'!1:1,0))</f>
+        <v>0.37801715742540049</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:AK3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2687,7 +6893,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="43.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="5">
@@ -2972,128 +7178,128 @@
         <v>21.196137258578663</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!C3</f>
+        <v>10.926216502206371</v>
       </c>
       <c r="H3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!D3</f>
+        <v>15.24360576579239</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!E3</f>
+        <v>17.407327883986987</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!F3</f>
+        <v>18.558042836824331</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!G3</f>
+        <v>19.224124239341972</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!H3</f>
+        <v>19.65155655886592</v>
       </c>
       <c r="M3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!I3</f>
+        <v>19.936314478020616</v>
       </c>
       <c r="N3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!J3</f>
+        <v>20.134691016987187</v>
       </c>
       <c r="O3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!K3</f>
+        <v>20.276277259192209</v>
       </c>
       <c r="P3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!L3</f>
+        <v>20.375704130653386</v>
       </c>
       <c r="Q3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!M3</f>
+        <v>20.448532051037215</v>
       </c>
       <c r="R3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!N3</f>
+        <v>20.494994831117225</v>
       </c>
       <c r="S3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!O3</f>
+        <v>20.538485652340103</v>
       </c>
       <c r="T3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!P3</f>
+        <v>20.56215722797787</v>
       </c>
       <c r="U3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!Q3</f>
+        <v>20.576566346449859</v>
       </c>
       <c r="V3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!R3</f>
+        <v>20.581322247213965</v>
       </c>
       <c r="W3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!S3</f>
+        <v>20.584869957535812</v>
       </c>
       <c r="X3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!T3</f>
+        <v>20.595754565201876</v>
       </c>
       <c r="Y3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!U3</f>
+        <v>20.599051317281923</v>
       </c>
       <c r="Z3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!V3</f>
+        <v>20.575955392241411</v>
       </c>
       <c r="AA3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!W3</f>
+        <v>20.555993015729808</v>
       </c>
       <c r="AB3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!X3</f>
+        <v>20.525003001493104</v>
       </c>
       <c r="AC3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!Y3</f>
+        <v>20.491448734674744</v>
       </c>
       <c r="AD3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!Z3</f>
+        <v>20.455193338130783</v>
       </c>
       <c r="AE3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AA3</f>
+        <v>20.414559083390188</v>
       </c>
       <c r="AF3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AB3</f>
+        <v>20.373675585154615</v>
       </c>
       <c r="AG3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AC3</f>
+        <v>20.333732474253587</v>
       </c>
       <c r="AH3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AD3</f>
+        <v>20.291445304437243</v>
       </c>
       <c r="AI3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AE3</f>
+        <v>20.246116778950924</v>
       </c>
       <c r="AJ3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AF3</f>
+        <v>20.198892146941517</v>
       </c>
       <c r="AK3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
+        <f>$B3*BCDTRtSY!AG3</f>
+        <v>20.148401426560067</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -3395,7 +7601,7 @@
       </c>
     </row>
     <row r="6" spans="1:37">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="7">
@@ -3696,7 +7902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -3711,7 +7917,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="43.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="1">
@@ -3824,7 +8030,7 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>1</v>
       </c>
       <c r="C2">

</xml_diff>

<commit_message>
Move to using start year versions of BAU avg annual dist traveled by veh type and avg vehicle loading, start year transport calibration
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B446D3AE-B87D-4E62-AC29-BC99054FBCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA62E737-16DD-479C-935A-B97ED393513D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BTS NTS Modal Profile Data" sheetId="3" r:id="rId2"/>
-    <sheet name="AVLo-passengers" sheetId="2" r:id="rId3"/>
-    <sheet name="AVLo-freight" sheetId="4" r:id="rId4"/>
+    <sheet name="SYAVLo-passengers" sheetId="2" r:id="rId3"/>
+    <sheet name="SYAVLo-freight" sheetId="4" r:id="rId4"/>
+    <sheet name="AVLo-passengers" sheetId="5" r:id="rId5"/>
+    <sheet name="AVLo-freight" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Eno_TM">'[1]1997  Table 1a Modified'!#REF!</definedName>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -1467,7 +1469,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Rail shipments 93-97"/>
@@ -1548,9 +1550,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1588,9 +1590,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1623,26 +1625,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1675,26 +1660,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1874,10 +1842,10 @@
       <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" customWidth="1"/>
-    <col min="2" max="2" width="85.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2149,11 +2117,11 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.6328125" customWidth="1"/>
+    <col min="1" max="1" width="73.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.26953125" customWidth="1"/>
+    <col min="3" max="3" width="102.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2672,280 +2640,35 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:AK3"/>
+      <selection activeCell="C1" sqref="C1:AK1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="43.5">
+    <row r="1" spans="1:2" ht="45">
       <c r="A1" s="16" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="5">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="5">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="5">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
         <v>2020</v>
       </c>
-      <c r="H1" s="5">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="5">
-        <v>2023</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L1" s="5">
-        <v>2025</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2026</v>
-      </c>
-      <c r="N1" s="5">
-        <v>2027</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2028</v>
-      </c>
-      <c r="P1" s="5">
-        <v>2029</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2030</v>
-      </c>
-      <c r="R1" s="5">
-        <v>2031</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2032</v>
-      </c>
-      <c r="T1" s="5">
-        <v>2033</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2034</v>
-      </c>
-      <c r="V1" s="5">
-        <v>2035</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2036</v>
-      </c>
-      <c r="X1" s="5">
-        <v>2037</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>2038</v>
-      </c>
-      <c r="Z1" s="5">
-        <v>2039</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>2040</v>
-      </c>
-      <c r="AB1" s="5">
-        <v>2041</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>2042</v>
-      </c>
-      <c r="AD1" s="5">
-        <v>2043</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>2044</v>
-      </c>
-      <c r="AF1" s="5">
-        <v>2045</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>2046</v>
-      </c>
-      <c r="AH1" s="5">
-        <v>2047</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AJ1" s="5">
-        <v>2049</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="7">
         <v>1.67</v>
       </c>
-      <c r="C2" s="7">
-        <f>$B2</f>
-        <v>1.67</v>
-      </c>
-      <c r="D2" s="7">
-        <f t="shared" ref="D2:AK7" si="0">$B2</f>
-        <v>1.67</v>
-      </c>
-      <c r="E2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="F2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="G2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="H2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="I2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="J2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="K2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="L2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="M2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="N2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="O2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="P2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="Q2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="R2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="S2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="T2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="U2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="V2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="W2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="X2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="Y2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="Z2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AA2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AB2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AC2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AD2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AE2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AF2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AG2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AH2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AI2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AJ2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="AK2" s="7">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2953,148 +2676,8 @@
         <f>'BTS NTS Modal Profile Data'!B14</f>
         <v>21.196137258578663</v>
       </c>
-      <c r="C3" s="7">
-        <f t="shared" ref="C3:R7" si="1">$B3</f>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="D3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="E3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="F3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="G3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="H3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="I3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="J3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="K3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="M3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="N3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="O3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="P3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="Q3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="R3" s="7">
-        <f t="shared" si="1"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="S3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="T3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="U3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="V3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="W3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="X3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="Y3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="Z3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AA3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AB3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AC3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AD3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AE3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AF3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AG3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AH3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AI3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AJ3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-      <c r="AK3" s="7">
-        <f t="shared" si="0"/>
-        <v>21.196137258578663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3102,148 +2685,8 @@
         <f>'BTS NTS Modal Profile Data'!B8</f>
         <v>111.39416306433705</v>
       </c>
-      <c r="C4" s="7">
-        <f t="shared" si="1"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="D4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="E4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="F4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="M4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="N4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="O4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="P4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="Q4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="R4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="S4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="T4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="U4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="V4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="W4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="X4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="Y4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="Z4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AA4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AB4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AC4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AD4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AE4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AF4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AG4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AH4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AI4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AJ4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-      <c r="AK4" s="7">
-        <f t="shared" si="0"/>
-        <v>111.39416306433705</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -3251,441 +2694,21 @@
         <f>'BTS NTS Modal Profile Data'!B37</f>
         <v>486.56731685074101</v>
       </c>
-      <c r="C5" s="7">
-        <f t="shared" si="1"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="L5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="M5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="N5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="O5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="P5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="Q5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="R5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="S5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="T5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="U5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="V5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="W5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="X5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="Y5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="Z5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AA5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AB5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AC5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AD5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AE5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AF5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AG5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AH5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AI5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AJ5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-      <c r="AK5" s="7">
-        <f t="shared" si="0"/>
-        <v>486.56731685074101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="X6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Y6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Z6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AA6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AC6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AD6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AE6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AF6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AG6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AH6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AI6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AK6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="7">
         <f>'BTS NTS Modal Profile Data'!B60</f>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="C7" s="7">
-        <f t="shared" si="1"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="E7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="F7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="H7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="I7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="J7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="K7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="N7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="O7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="P7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="Q7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="S7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="T7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="U7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="V7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="W7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="X7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="Y7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="Z7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AA7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AB7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AC7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AD7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AE7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AF7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AG7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AH7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AI7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AJ7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2700756740871355</v>
-      </c>
-      <c r="AK7" s="7">
-        <f t="shared" si="0"/>
         <v>1.2700756740871355</v>
       </c>
     </row>
@@ -3699,414 +2722,42 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="43.5">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="45">
       <c r="A1" s="16" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="1">
         <v>2020</v>
       </c>
-      <c r="G1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2023</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2024</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2025</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2026</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2027</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2028</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2029</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2030</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2031</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2032</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2033</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2034</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2035</v>
-      </c>
-      <c r="V1" s="1">
-        <v>2036</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2037</v>
-      </c>
-      <c r="X1" s="1">
-        <v>2038</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>2039</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>2040</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>2041</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>2042</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>2043</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>2044</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>2045</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>2046</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>2047</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>2049</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:R7" si="0">$B2</f>
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <f t="shared" ref="D2:AJ7" si="1">$B2</f>
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AH2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AI2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="6">
         <v>16</v>
       </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="R3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="S3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="T3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="V3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="W3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="X3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="Z3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AA3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AB3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AC3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AD3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AE3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AF3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AG3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AH3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AI3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AJ3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -4114,144 +2765,8 @@
         <f>'BTS NTS Modal Profile Data'!B9</f>
         <v>41.989116133258747</v>
       </c>
-      <c r="C4" s="6">
-        <f t="shared" si="0"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="D4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="E4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="F4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="G4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="H4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="I4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="J4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="L4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="M4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="N4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="O4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="P4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="Q4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="R4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="S4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="T4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="U4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="V4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="W4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="X4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="Y4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="Z4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AA4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AB4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AC4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AD4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AE4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AF4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AG4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AH4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AI4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-      <c r="AJ4" s="6">
-        <f t="shared" si="1"/>
-        <v>41.989116133258747</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -4259,144 +2774,8 @@
         <f>'BTS NTS Modal Profile Data'!B19</f>
         <v>3512.35916421195</v>
       </c>
-      <c r="C5" s="6">
-        <f t="shared" si="0"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="D5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="E5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="F5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="G5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="H5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="I5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="J5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="K5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="L5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="M5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="N5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="O5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="P5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="Q5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="R5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="S5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="T5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="U5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="V5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="W5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="X5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="Z5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AA5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AB5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AC5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AD5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AE5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AF5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AG5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AH5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AI5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-      <c r="AJ5" s="6">
-        <f t="shared" si="1"/>
-        <v>3512.35916421195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -4404,284 +2783,1741 @@
         <f>'BTS NTS Modal Profile Data'!B55</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="C6" s="6">
-        <f t="shared" si="0"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="D6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="E6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="G6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="J6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="K6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="L6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="M6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="N6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="O6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="P6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="Q6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="R6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="S6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="T6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="U6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="V6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="X6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="Y6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="Z6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AA6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AB6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AC6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AD6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AE6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AF6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AG6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AH6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AI6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-      <c r="AJ6" s="6">
-        <f t="shared" si="1"/>
-        <v>1974.4736422180429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A6C762-134A-444D-BF60-BC99F3DFC165}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AE7"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="45">
+      <c r="A1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="5">
+        <v>2024</v>
+      </c>
+      <c r="F1" s="5">
+        <v>2025</v>
+      </c>
+      <c r="G1" s="5">
+        <v>2026</v>
+      </c>
+      <c r="H1" s="5">
+        <v>2027</v>
+      </c>
+      <c r="I1" s="5">
+        <v>2028</v>
+      </c>
+      <c r="J1" s="5">
+        <v>2029</v>
+      </c>
+      <c r="K1" s="5">
+        <v>2030</v>
+      </c>
+      <c r="L1" s="5">
+        <v>2031</v>
+      </c>
+      <c r="M1" s="5">
+        <v>2032</v>
+      </c>
+      <c r="N1" s="5">
+        <v>2033</v>
+      </c>
+      <c r="O1" s="5">
+        <v>2034</v>
+      </c>
+      <c r="P1" s="5">
+        <v>2035</v>
+      </c>
+      <c r="Q1" s="5">
+        <v>2036</v>
+      </c>
+      <c r="R1" s="5">
+        <v>2037</v>
+      </c>
+      <c r="S1" s="5">
+        <v>2038</v>
+      </c>
+      <c r="T1" s="5">
+        <v>2039</v>
+      </c>
+      <c r="U1" s="5">
+        <v>2040</v>
+      </c>
+      <c r="V1" s="5">
+        <v>2041</v>
+      </c>
+      <c r="W1" s="5">
+        <v>2042</v>
+      </c>
+      <c r="X1" s="5">
+        <v>2043</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>2044</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>2046</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AC1" s="5">
+        <v>2048</v>
+      </c>
+      <c r="AD1" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AE1" s="5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="C2" s="7">
+        <f>$B2</f>
+        <v>1.67</v>
+      </c>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:AE7" si="0">$B2</f>
+        <v>1.67</v>
+      </c>
+      <c r="E2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="F2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="G2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="H2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="J2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="K2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="L2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="M2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="N2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="O2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="P2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="Q2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="R2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="S2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="T2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="U2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="V2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="W2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="X2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="Y2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="Z2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="AA2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="AB2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="AC2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="AD2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+      <c r="AE2" s="7">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9">
+        <f>'BTS NTS Modal Profile Data'!B14</f>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:R7" si="1">$B3</f>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="M3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="N3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="R3" s="7">
+        <f t="shared" si="1"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="S3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="T3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="U3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="V3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="W3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="X3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Y3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Z3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AA3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AB3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AC3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AD3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AE3" s="7">
+        <f t="shared" si="0"/>
+        <v>21.196137258578663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9">
+        <f>'BTS NTS Modal Profile Data'!B8</f>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="1"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="S4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="T4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="W4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="X4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Y4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Z4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AA4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AB4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AC4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AD4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AE4" s="7">
+        <f t="shared" si="0"/>
+        <v>111.39416306433705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9">
+        <f>'BTS NTS Modal Profile Data'!B37</f>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="1"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="M5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="N5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Q5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="S5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="T5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="U5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="V5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="W5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="X5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Y5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Z5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AA5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AB5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AC5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AD5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AE5" s="7">
+        <f t="shared" si="0"/>
+        <v>486.56731685074101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7">
+        <f>'BTS NTS Modal Profile Data'!B60</f>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="N7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="T7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="V7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="W7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="X7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Y7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Z7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AA7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AB7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AC7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AD7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AE7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2700756740871355</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87475B98-F0F0-452D-A62B-4E672A3FB155}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AE7"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1:AJ1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="45">
+      <c r="A1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:F7" si="0">$B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <f>$B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="P3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="Q3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="S3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="T3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="U3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="V3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="W3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="X3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="Y3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="Z3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="AA3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="AB3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="AC3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="AD3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+      <c r="AE3">
+        <f>$B3</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <f>'BTS NTS Modal Profile Data'!B9</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="G4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="H4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="I4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="J4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="K4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="L4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="M4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="N4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="O4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="P4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Q4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="R4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="S4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="T4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="U4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="V4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="W4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="X4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Y4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Z4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AA4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AB4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AC4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AD4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AE4" s="6">
+        <f>$B4</f>
+        <v>41.989116133258747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6">
+        <f>'BTS NTS Modal Profile Data'!B19</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="G5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="H5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="I5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="J5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="K5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="L5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="M5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="N5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="O5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="P5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="R5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="S5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="T5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="U5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="V5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="W5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="X5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Y5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Z5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AA5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AB5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AC5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AD5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AE5" s="6">
+        <f>$B5</f>
+        <v>3512.35916421195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6">
+        <f>'BTS NTS Modal Profile Data'!B55</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="G6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="H6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="I6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="J6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="K6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="L6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="M6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="N6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="O6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="P6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="R6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="S6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="T6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="U6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="V6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="W6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="X6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Y6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Z6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AA6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AB6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AC6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AD6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AE6" s="6">
+        <f>$B6</f>
+        <v>1974.4736422180429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="S7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <f t="shared" si="1"/>
+        <f>$B7</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>